<commit_message>
add hibernate gen table from class added id in token table
</commit_message>
<xml_diff>
--- a/doc/backend/db/TRN-MiniBlog_DatabaseDesign_LeDangHuy.xlsx
+++ b/doc/backend/db/TRN-MiniBlog_DatabaseDesign_LeDangHuy.xlsx
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="197">
   <si>
     <t>No</t>
   </si>
@@ -3381,7 +3381,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="318">
+  <cellXfs count="324">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3934,6 +3934,168 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3944,12 +4106,75 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="16" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3965,69 +4190,6 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4052,9 +4214,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="29" fillId="2" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4073,10 +4232,22 @@
     <xf numFmtId="49" fontId="29" fillId="2" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="29" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4085,16 +4256,10 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4103,194 +4268,47 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="23" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="23" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="64" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="444">
@@ -6014,29 +6032,29 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="198"/>
-      <c r="P13" s="198"/>
-      <c r="Q13" s="198"/>
-      <c r="R13" s="198"/>
-      <c r="S13" s="198"/>
-      <c r="T13" s="198"/>
-      <c r="U13" s="198"/>
-      <c r="V13" s="198"/>
-      <c r="W13" s="198"/>
-      <c r="X13" s="198"/>
-      <c r="Y13" s="198"/>
-      <c r="Z13" s="198"/>
-      <c r="AA13" s="198"/>
-      <c r="AB13" s="198"/>
-      <c r="AC13" s="198"/>
-      <c r="AD13" s="198"/>
-      <c r="AE13" s="198"/>
-      <c r="AF13" s="198"/>
-      <c r="AG13" s="198"/>
-      <c r="AH13" s="198"/>
-      <c r="AI13" s="198"/>
-      <c r="AJ13" s="198"/>
-      <c r="AK13" s="198"/>
+      <c r="O13" s="252"/>
+      <c r="P13" s="252"/>
+      <c r="Q13" s="252"/>
+      <c r="R13" s="252"/>
+      <c r="S13" s="252"/>
+      <c r="T13" s="252"/>
+      <c r="U13" s="252"/>
+      <c r="V13" s="252"/>
+      <c r="W13" s="252"/>
+      <c r="X13" s="252"/>
+      <c r="Y13" s="252"/>
+      <c r="Z13" s="252"/>
+      <c r="AA13" s="252"/>
+      <c r="AB13" s="252"/>
+      <c r="AC13" s="252"/>
+      <c r="AD13" s="252"/>
+      <c r="AE13" s="252"/>
+      <c r="AF13" s="252"/>
+      <c r="AG13" s="252"/>
+      <c r="AH13" s="252"/>
+      <c r="AI13" s="252"/>
+      <c r="AJ13" s="252"/>
+      <c r="AK13" s="252"/>
       <c r="AL13" s="4"/>
       <c r="AM13" s="4"/>
       <c r="AN13" s="4"/>
@@ -6068,29 +6086,29 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="198"/>
-      <c r="P14" s="198"/>
-      <c r="Q14" s="198"/>
-      <c r="R14" s="198"/>
-      <c r="S14" s="198"/>
-      <c r="T14" s="198"/>
-      <c r="U14" s="198"/>
-      <c r="V14" s="198"/>
-      <c r="W14" s="198"/>
-      <c r="X14" s="198"/>
-      <c r="Y14" s="198"/>
-      <c r="Z14" s="198"/>
-      <c r="AA14" s="198"/>
-      <c r="AB14" s="198"/>
-      <c r="AC14" s="198"/>
-      <c r="AD14" s="198"/>
-      <c r="AE14" s="198"/>
-      <c r="AF14" s="198"/>
-      <c r="AG14" s="198"/>
-      <c r="AH14" s="198"/>
-      <c r="AI14" s="198"/>
-      <c r="AJ14" s="198"/>
-      <c r="AK14" s="198"/>
+      <c r="O14" s="252"/>
+      <c r="P14" s="252"/>
+      <c r="Q14" s="252"/>
+      <c r="R14" s="252"/>
+      <c r="S14" s="252"/>
+      <c r="T14" s="252"/>
+      <c r="U14" s="252"/>
+      <c r="V14" s="252"/>
+      <c r="W14" s="252"/>
+      <c r="X14" s="252"/>
+      <c r="Y14" s="252"/>
+      <c r="Z14" s="252"/>
+      <c r="AA14" s="252"/>
+      <c r="AB14" s="252"/>
+      <c r="AC14" s="252"/>
+      <c r="AD14" s="252"/>
+      <c r="AE14" s="252"/>
+      <c r="AF14" s="252"/>
+      <c r="AG14" s="252"/>
+      <c r="AH14" s="252"/>
+      <c r="AI14" s="252"/>
+      <c r="AJ14" s="252"/>
+      <c r="AK14" s="252"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
@@ -6118,43 +6136,43 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="199" t="s">
+      <c r="K15" s="253" t="s">
         <v>119</v>
       </c>
-      <c r="L15" s="199"/>
-      <c r="M15" s="199"/>
-      <c r="N15" s="199"/>
-      <c r="O15" s="199"/>
-      <c r="P15" s="199"/>
-      <c r="Q15" s="199"/>
-      <c r="R15" s="199"/>
-      <c r="S15" s="199"/>
-      <c r="T15" s="199"/>
-      <c r="U15" s="199"/>
-      <c r="V15" s="199"/>
-      <c r="W15" s="199"/>
-      <c r="X15" s="199"/>
-      <c r="Y15" s="199"/>
-      <c r="Z15" s="199"/>
-      <c r="AA15" s="199"/>
-      <c r="AB15" s="199"/>
-      <c r="AC15" s="199"/>
-      <c r="AD15" s="199"/>
-      <c r="AE15" s="199"/>
-      <c r="AF15" s="199"/>
-      <c r="AG15" s="199"/>
-      <c r="AH15" s="199"/>
-      <c r="AI15" s="199"/>
-      <c r="AJ15" s="199"/>
-      <c r="AK15" s="199"/>
-      <c r="AL15" s="199"/>
-      <c r="AM15" s="199"/>
-      <c r="AN15" s="199"/>
-      <c r="AO15" s="199"/>
-      <c r="AP15" s="199"/>
-      <c r="AQ15" s="199"/>
-      <c r="AR15" s="199"/>
-      <c r="AS15" s="199"/>
+      <c r="L15" s="253"/>
+      <c r="M15" s="253"/>
+      <c r="N15" s="253"/>
+      <c r="O15" s="253"/>
+      <c r="P15" s="253"/>
+      <c r="Q15" s="253"/>
+      <c r="R15" s="253"/>
+      <c r="S15" s="253"/>
+      <c r="T15" s="253"/>
+      <c r="U15" s="253"/>
+      <c r="V15" s="253"/>
+      <c r="W15" s="253"/>
+      <c r="X15" s="253"/>
+      <c r="Y15" s="253"/>
+      <c r="Z15" s="253"/>
+      <c r="AA15" s="253"/>
+      <c r="AB15" s="253"/>
+      <c r="AC15" s="253"/>
+      <c r="AD15" s="253"/>
+      <c r="AE15" s="253"/>
+      <c r="AF15" s="253"/>
+      <c r="AG15" s="253"/>
+      <c r="AH15" s="253"/>
+      <c r="AI15" s="253"/>
+      <c r="AJ15" s="253"/>
+      <c r="AK15" s="253"/>
+      <c r="AL15" s="253"/>
+      <c r="AM15" s="253"/>
+      <c r="AN15" s="253"/>
+      <c r="AO15" s="253"/>
+      <c r="AP15" s="253"/>
+      <c r="AQ15" s="253"/>
+      <c r="AR15" s="253"/>
+      <c r="AS15" s="253"/>
       <c r="AT15" s="4"/>
       <c r="AU15" s="4"/>
       <c r="AV15" s="4"/>
@@ -6174,41 +6192,41 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="199"/>
-      <c r="L16" s="199"/>
-      <c r="M16" s="199"/>
-      <c r="N16" s="199"/>
-      <c r="O16" s="199"/>
-      <c r="P16" s="199"/>
-      <c r="Q16" s="199"/>
-      <c r="R16" s="199"/>
-      <c r="S16" s="199"/>
-      <c r="T16" s="199"/>
-      <c r="U16" s="199"/>
-      <c r="V16" s="199"/>
-      <c r="W16" s="199"/>
-      <c r="X16" s="199"/>
-      <c r="Y16" s="199"/>
-      <c r="Z16" s="199"/>
-      <c r="AA16" s="199"/>
-      <c r="AB16" s="199"/>
-      <c r="AC16" s="199"/>
-      <c r="AD16" s="199"/>
-      <c r="AE16" s="199"/>
-      <c r="AF16" s="199"/>
-      <c r="AG16" s="199"/>
-      <c r="AH16" s="199"/>
-      <c r="AI16" s="199"/>
-      <c r="AJ16" s="199"/>
-      <c r="AK16" s="199"/>
-      <c r="AL16" s="199"/>
-      <c r="AM16" s="199"/>
-      <c r="AN16" s="199"/>
-      <c r="AO16" s="199"/>
-      <c r="AP16" s="199"/>
-      <c r="AQ16" s="199"/>
-      <c r="AR16" s="199"/>
-      <c r="AS16" s="199"/>
+      <c r="K16" s="253"/>
+      <c r="L16" s="253"/>
+      <c r="M16" s="253"/>
+      <c r="N16" s="253"/>
+      <c r="O16" s="253"/>
+      <c r="P16" s="253"/>
+      <c r="Q16" s="253"/>
+      <c r="R16" s="253"/>
+      <c r="S16" s="253"/>
+      <c r="T16" s="253"/>
+      <c r="U16" s="253"/>
+      <c r="V16" s="253"/>
+      <c r="W16" s="253"/>
+      <c r="X16" s="253"/>
+      <c r="Y16" s="253"/>
+      <c r="Z16" s="253"/>
+      <c r="AA16" s="253"/>
+      <c r="AB16" s="253"/>
+      <c r="AC16" s="253"/>
+      <c r="AD16" s="253"/>
+      <c r="AE16" s="253"/>
+      <c r="AF16" s="253"/>
+      <c r="AG16" s="253"/>
+      <c r="AH16" s="253"/>
+      <c r="AI16" s="253"/>
+      <c r="AJ16" s="253"/>
+      <c r="AK16" s="253"/>
+      <c r="AL16" s="253"/>
+      <c r="AM16" s="253"/>
+      <c r="AN16" s="253"/>
+      <c r="AO16" s="253"/>
+      <c r="AP16" s="253"/>
+      <c r="AQ16" s="253"/>
+      <c r="AR16" s="253"/>
+      <c r="AS16" s="253"/>
       <c r="AT16" s="4"/>
       <c r="AU16" s="4"/>
       <c r="AV16" s="4"/>
@@ -6797,14 +6815,14 @@
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
       <c r="AM27" s="7"/>
-      <c r="AN27" s="200">
+      <c r="AN27" s="254">
         <v>41922</v>
       </c>
-      <c r="AO27" s="200"/>
-      <c r="AP27" s="200"/>
-      <c r="AQ27" s="200"/>
-      <c r="AR27" s="200"/>
-      <c r="AS27" s="200"/>
+      <c r="AO27" s="254"/>
+      <c r="AP27" s="254"/>
+      <c r="AQ27" s="254"/>
+      <c r="AR27" s="254"/>
+      <c r="AS27" s="254"/>
       <c r="AT27" s="12"/>
       <c r="AU27" s="12"/>
       <c r="AV27" s="12"/>
@@ -7294,103 +7312,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="256" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="228"/>
+      <c r="D2" s="257"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="255" t="s">
+      <c r="F2" s="312" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="256"/>
+      <c r="G2" s="313"/>
     </row>
     <row r="3" spans="1:14" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
+      <c r="C3" s="258"/>
+      <c r="D3" s="259"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="225" t="s">
+      <c r="F3" s="261" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="226"/>
+      <c r="G3" s="262"/>
     </row>
     <row r="4" spans="1:14" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="227" t="s">
+      <c r="C4" s="258" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="229"/>
+      <c r="D4" s="259"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="226"/>
+      <c r="F4" s="258"/>
+      <c r="G4" s="262"/>
     </row>
     <row r="5" spans="1:14" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="258" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="229"/>
+      <c r="D5" s="259"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="226"/>
+      <c r="F5" s="258"/>
+      <c r="G5" s="262"/>
     </row>
     <row r="6" spans="1:14" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="258" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="229"/>
+      <c r="D6" s="259"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="226"/>
+      <c r="F6" s="258"/>
+      <c r="G6" s="262"/>
     </row>
     <row r="7" spans="1:14" ht="14.25">
-      <c r="B7" s="211" t="s">
+      <c r="B7" s="267" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="212"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="213"/>
+      <c r="C7" s="268"/>
+      <c r="D7" s="268"/>
+      <c r="E7" s="268"/>
+      <c r="F7" s="268"/>
+      <c r="G7" s="269"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="214"/>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
+      <c r="B8" s="270"/>
+      <c r="C8" s="271"/>
+      <c r="D8" s="271"/>
+      <c r="E8" s="271"/>
+      <c r="F8" s="271"/>
+      <c r="G8" s="272"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="217"/>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="216"/>
+      <c r="B9" s="273"/>
+      <c r="C9" s="271"/>
+      <c r="D9" s="271"/>
+      <c r="E9" s="271"/>
+      <c r="F9" s="271"/>
+      <c r="G9" s="272"/>
     </row>
     <row r="10" spans="1:14" ht="12.75" thickBot="1">
-      <c r="B10" s="218"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="220"/>
+      <c r="B10" s="274"/>
+      <c r="C10" s="275"/>
+      <c r="D10" s="275"/>
+      <c r="E10" s="275"/>
+      <c r="F10" s="275"/>
+      <c r="G10" s="276"/>
     </row>
     <row r="11" spans="1:14">
       <c r="H11" s="87"/>
@@ -7606,10 +7624,10 @@
       <c r="B21" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="209" t="s">
+      <c r="C21" s="263" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="210"/>
+      <c r="D21" s="264"/>
       <c r="E21" s="34" t="s">
         <v>33</v>
       </c>
@@ -7633,10 +7651,10 @@
       <c r="B22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="249" t="s">
+      <c r="C22" s="302" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="250"/>
+      <c r="D22" s="303"/>
       <c r="E22" s="46" t="s">
         <v>3</v>
       </c>
@@ -7656,10 +7674,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="253" t="s">
+      <c r="C23" s="308" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="254"/>
+      <c r="D23" s="309"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
         <v>3</v>
@@ -7677,10 +7695,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="26"/>
-      <c r="C24" s="245" t="s">
+      <c r="C24" s="306" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="246"/>
+      <c r="D24" s="307"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45" t="s">
         <v>3</v>
@@ -7719,14 +7737,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="202" t="s">
+      <c r="C27" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="203"/>
-      <c r="E27" s="202" t="s">
+      <c r="D27" s="266"/>
+      <c r="E27" s="265" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="204"/>
+      <c r="F27" s="279"/>
       <c r="G27" s="38" t="s">
         <v>38</v>
       </c>
@@ -7763,14 +7781,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="202" t="s">
+      <c r="C30" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="203"/>
-      <c r="E30" s="202" t="s">
+      <c r="D30" s="266"/>
+      <c r="E30" s="265" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="204"/>
+      <c r="F30" s="279"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
@@ -7786,14 +7804,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="249" t="s">
+      <c r="C31" s="302" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="250"/>
-      <c r="E31" s="253" t="s">
+      <c r="D31" s="303"/>
+      <c r="E31" s="308" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="254"/>
+      <c r="F31" s="309"/>
       <c r="G31" s="53" t="s">
         <v>76</v>
       </c>
@@ -7809,14 +7827,14 @@
         <v>2</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="251" t="s">
+      <c r="C32" s="310" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="252"/>
-      <c r="E32" s="247" t="s">
+      <c r="D32" s="311"/>
+      <c r="E32" s="304" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="248"/>
+      <c r="F32" s="305"/>
       <c r="G32" s="55" t="s">
         <v>52</v>
       </c>
@@ -7869,14 +7887,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="C31:D31"/>
@@ -7893,6 +7903,14 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8209,11 +8227,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" thickBot="1">
-      <c r="A1" s="201" t="s">
+      <c r="A1" s="255" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
+      <c r="B1" s="255"/>
+      <c r="C1" s="255"/>
     </row>
     <row r="2" spans="1:3" ht="12.75" thickBot="1">
       <c r="A2" s="118" t="s">
@@ -8508,103 +8526,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="256" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="228"/>
+      <c r="D2" s="257"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="223" t="s">
+      <c r="F2" s="256" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="224"/>
+      <c r="G2" s="260"/>
     </row>
     <row r="3" spans="1:19" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
+      <c r="C3" s="258"/>
+      <c r="D3" s="259"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="225" t="s">
+      <c r="F3" s="261" t="s">
         <v>150</v>
       </c>
-      <c r="G3" s="226"/>
+      <c r="G3" s="262"/>
     </row>
     <row r="4" spans="1:19" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="227" t="s">
+      <c r="C4" s="258" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="229"/>
+      <c r="D4" s="259"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="226"/>
+      <c r="F4" s="258"/>
+      <c r="G4" s="262"/>
     </row>
     <row r="5" spans="1:19" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="258" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="229"/>
+      <c r="D5" s="259"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="226"/>
+      <c r="F5" s="258"/>
+      <c r="G5" s="262"/>
     </row>
     <row r="6" spans="1:19" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="258" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="229"/>
+      <c r="D6" s="259"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="226"/>
+      <c r="F6" s="258"/>
+      <c r="G6" s="262"/>
     </row>
     <row r="7" spans="1:19" ht="14.25">
-      <c r="B7" s="211" t="s">
+      <c r="B7" s="267" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="212"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="213"/>
+      <c r="C7" s="268"/>
+      <c r="D7" s="268"/>
+      <c r="E7" s="268"/>
+      <c r="F7" s="268"/>
+      <c r="G7" s="269"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="214"/>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
+      <c r="B8" s="270"/>
+      <c r="C8" s="271"/>
+      <c r="D8" s="271"/>
+      <c r="E8" s="271"/>
+      <c r="F8" s="271"/>
+      <c r="G8" s="272"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="217"/>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="216"/>
+      <c r="B9" s="273"/>
+      <c r="C9" s="271"/>
+      <c r="D9" s="271"/>
+      <c r="E9" s="271"/>
+      <c r="F9" s="271"/>
+      <c r="G9" s="272"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" thickBot="1">
-      <c r="B10" s="218"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="220"/>
+      <c r="B10" s="274"/>
+      <c r="C10" s="275"/>
+      <c r="D10" s="275"/>
+      <c r="E10" s="275"/>
+      <c r="F10" s="275"/>
+      <c r="G10" s="276"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8922,10 +8940,10 @@
       <c r="B25" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="209" t="s">
+      <c r="C25" s="263" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="210"/>
+      <c r="D25" s="264"/>
       <c r="E25" s="34" t="s">
         <v>33</v>
       </c>
@@ -8943,10 +8961,10 @@
       <c r="B26" s="166" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="221" t="s">
+      <c r="C26" s="277" t="s">
         <v>114</v>
       </c>
-      <c r="D26" s="222"/>
+      <c r="D26" s="278"/>
       <c r="E26" s="167" t="s">
         <v>3</v>
       </c>
@@ -8962,10 +8980,10 @@
       <c r="B27" s="155" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="207" t="s">
+      <c r="C27" s="282" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="208"/>
+      <c r="D27" s="283"/>
       <c r="E27" s="169"/>
       <c r="F27" s="44" t="s">
         <v>3</v>
@@ -8994,8 +9012,8 @@
     <row r="29" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
       <c r="A29" s="16"/>
       <c r="B29" s="172"/>
-      <c r="C29" s="205"/>
-      <c r="D29" s="206"/>
+      <c r="C29" s="280"/>
+      <c r="D29" s="281"/>
       <c r="E29" s="45"/>
       <c r="F29" s="45"/>
       <c r="G29" s="28"/>
@@ -9012,14 +9030,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="202" t="s">
+      <c r="C32" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="203"/>
-      <c r="E32" s="202" t="s">
+      <c r="D32" s="266"/>
+      <c r="E32" s="265" t="s">
         <v>36</v>
       </c>
-      <c r="F32" s="204"/>
+      <c r="F32" s="279"/>
       <c r="G32" s="38" t="s">
         <v>38</v>
       </c>
@@ -9036,40 +9054,40 @@
       <c r="B35" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="202" t="s">
+      <c r="C35" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="203"/>
-      <c r="E35" s="202" t="s">
+      <c r="D35" s="266"/>
+      <c r="E35" s="265" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="204"/>
+      <c r="F35" s="279"/>
       <c r="G35" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9122,103 +9140,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="256" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="228"/>
+      <c r="D2" s="257"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="223" t="s">
+      <c r="F2" s="256" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="224"/>
+      <c r="G2" s="260"/>
     </row>
     <row r="3" spans="1:19" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
+      <c r="C3" s="258"/>
+      <c r="D3" s="259"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="225" t="s">
+      <c r="F3" s="261" t="s">
         <v>150</v>
       </c>
-      <c r="G3" s="226"/>
+      <c r="G3" s="262"/>
     </row>
     <row r="4" spans="1:19" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="227" t="s">
+      <c r="C4" s="258" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="229"/>
+      <c r="D4" s="259"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="226"/>
+      <c r="F4" s="258"/>
+      <c r="G4" s="262"/>
     </row>
     <row r="5" spans="1:19" ht="14.25">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="258" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="229"/>
+      <c r="D5" s="259"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="226"/>
+      <c r="F5" s="258"/>
+      <c r="G5" s="262"/>
     </row>
     <row r="6" spans="1:19" ht="14.25">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="258" t="s">
         <v>129</v>
       </c>
-      <c r="D6" s="229"/>
+      <c r="D6" s="259"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="226"/>
+      <c r="F6" s="258"/>
+      <c r="G6" s="262"/>
     </row>
     <row r="7" spans="1:19" ht="14.25">
-      <c r="B7" s="211" t="s">
+      <c r="B7" s="267" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="212"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="213"/>
+      <c r="C7" s="268"/>
+      <c r="D7" s="268"/>
+      <c r="E7" s="268"/>
+      <c r="F7" s="268"/>
+      <c r="G7" s="269"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="214"/>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
+      <c r="B8" s="270"/>
+      <c r="C8" s="271"/>
+      <c r="D8" s="271"/>
+      <c r="E8" s="271"/>
+      <c r="F8" s="271"/>
+      <c r="G8" s="272"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="217"/>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="216"/>
+      <c r="B9" s="273"/>
+      <c r="C9" s="271"/>
+      <c r="D9" s="271"/>
+      <c r="E9" s="271"/>
+      <c r="F9" s="271"/>
+      <c r="G9" s="272"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" thickBot="1">
-      <c r="B10" s="218"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="220"/>
+      <c r="B10" s="274"/>
+      <c r="C10" s="275"/>
+      <c r="D10" s="275"/>
+      <c r="E10" s="275"/>
+      <c r="F10" s="275"/>
+      <c r="G10" s="276"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9546,10 +9564,10 @@
       <c r="B27" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="209" t="s">
+      <c r="C27" s="263" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="210"/>
+      <c r="D27" s="264"/>
       <c r="E27" s="34" t="s">
         <v>33</v>
       </c>
@@ -9567,10 +9585,10 @@
       <c r="B28" s="186" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="230" t="s">
+      <c r="C28" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="D28" s="231"/>
+      <c r="D28" s="285"/>
       <c r="E28" s="187" t="s">
         <v>3</v>
       </c>
@@ -9586,10 +9604,10 @@
       <c r="B29" s="191" t="s">
         <v>154</v>
       </c>
-      <c r="C29" s="232" t="s">
+      <c r="C29" s="286" t="s">
         <v>154</v>
       </c>
-      <c r="D29" s="233"/>
+      <c r="D29" s="287"/>
       <c r="E29" s="192"/>
       <c r="F29" s="192"/>
       <c r="G29" s="193"/>
@@ -9601,10 +9619,10 @@
       <c r="B30" s="195" t="s">
         <v>165</v>
       </c>
-      <c r="C30" s="234" t="s">
+      <c r="C30" s="288" t="s">
         <v>159</v>
       </c>
-      <c r="D30" s="235"/>
+      <c r="D30" s="289"/>
       <c r="E30" s="196" t="s">
         <v>3</v>
       </c>
@@ -9628,14 +9646,14 @@
       <c r="B34" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="202" t="s">
+      <c r="C34" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="203"/>
-      <c r="E34" s="202" t="s">
+      <c r="D34" s="266"/>
+      <c r="E34" s="265" t="s">
         <v>36</v>
       </c>
-      <c r="F34" s="204"/>
+      <c r="F34" s="279"/>
       <c r="G34" s="38" t="s">
         <v>38</v>
       </c>
@@ -9649,10 +9667,10 @@
       </c>
       <c r="C35" s="174"/>
       <c r="D35" s="174"/>
-      <c r="E35" s="236" t="s">
+      <c r="E35" s="290" t="s">
         <v>167</v>
       </c>
-      <c r="F35" s="237"/>
+      <c r="F35" s="291"/>
       <c r="G35" s="175"/>
     </row>
     <row r="37" spans="1:7" ht="12.75" thickBot="1">
@@ -9667,29 +9685,20 @@
       <c r="B38" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="202" t="s">
+      <c r="C38" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="203"/>
-      <c r="E38" s="202" t="s">
+      <c r="D38" s="266"/>
+      <c r="E38" s="265" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="204"/>
+      <c r="F38" s="279"/>
       <c r="G38" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -9702,6 +9711,15 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9744,103 +9762,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="256" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="228"/>
+      <c r="D2" s="257"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="223" t="s">
+      <c r="F2" s="256" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="224"/>
+      <c r="G2" s="260"/>
     </row>
     <row r="3" spans="1:19" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
+      <c r="C3" s="258"/>
+      <c r="D3" s="259"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="238" t="s">
+      <c r="F3" s="298" t="s">
         <v>150</v>
       </c>
-      <c r="G3" s="226"/>
+      <c r="G3" s="262"/>
     </row>
     <row r="4" spans="1:19" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="227" t="s">
+      <c r="C4" s="258" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="229"/>
+      <c r="D4" s="259"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="226"/>
+      <c r="F4" s="258"/>
+      <c r="G4" s="262"/>
     </row>
     <row r="5" spans="1:19" ht="14.25">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="258" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="229"/>
+      <c r="D5" s="259"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="226"/>
+      <c r="F5" s="258"/>
+      <c r="G5" s="262"/>
     </row>
     <row r="6" spans="1:19" ht="14.25">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="258" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="229"/>
+      <c r="D6" s="259"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="226"/>
+      <c r="F6" s="258"/>
+      <c r="G6" s="262"/>
     </row>
     <row r="7" spans="1:19" ht="14.25">
-      <c r="B7" s="211" t="s">
+      <c r="B7" s="267" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="212"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="213"/>
+      <c r="C7" s="268"/>
+      <c r="D7" s="268"/>
+      <c r="E7" s="268"/>
+      <c r="F7" s="268"/>
+      <c r="G7" s="269"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="214"/>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
+      <c r="B8" s="270"/>
+      <c r="C8" s="271"/>
+      <c r="D8" s="271"/>
+      <c r="E8" s="271"/>
+      <c r="F8" s="271"/>
+      <c r="G8" s="272"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="217"/>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="216"/>
+      <c r="B9" s="273"/>
+      <c r="C9" s="271"/>
+      <c r="D9" s="271"/>
+      <c r="E9" s="271"/>
+      <c r="F9" s="271"/>
+      <c r="G9" s="272"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" thickBot="1">
-      <c r="B10" s="218"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="220"/>
+      <c r="B10" s="274"/>
+      <c r="C10" s="275"/>
+      <c r="D10" s="275"/>
+      <c r="E10" s="275"/>
+      <c r="F10" s="275"/>
+      <c r="G10" s="276"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -10110,10 +10128,10 @@
       <c r="B22" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="209" t="s">
+      <c r="C22" s="263" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="210"/>
+      <c r="D22" s="264"/>
       <c r="E22" s="34" t="s">
         <v>33</v>
       </c>
@@ -10131,10 +10149,10 @@
       <c r="B23" s="166" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="221" t="s">
+      <c r="C23" s="277" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="222"/>
+      <c r="D23" s="278"/>
       <c r="E23" s="167" t="s">
         <v>3</v>
       </c>
@@ -10150,10 +10168,10 @@
       <c r="B24" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="C24" s="207" t="s">
+      <c r="C24" s="282" t="s">
         <v>171</v>
       </c>
-      <c r="D24" s="208"/>
+      <c r="D24" s="283"/>
       <c r="E24" s="44"/>
       <c r="F24" s="44"/>
       <c r="G24" s="24"/>
@@ -10165,10 +10183,10 @@
       <c r="B25" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="C25" s="205" t="s">
+      <c r="C25" s="280" t="s">
         <v>159</v>
       </c>
-      <c r="D25" s="206"/>
+      <c r="D25" s="281"/>
       <c r="E25" s="45"/>
       <c r="F25" s="45"/>
       <c r="G25" s="28"/>
@@ -10185,14 +10203,14 @@
       <c r="B28" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="202" t="s">
+      <c r="C28" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="203"/>
-      <c r="E28" s="202" t="s">
+      <c r="D28" s="266"/>
+      <c r="E28" s="265" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="204"/>
+      <c r="F28" s="279"/>
       <c r="G28" s="38" t="s">
         <v>38</v>
       </c>
@@ -10204,12 +10222,12 @@
       <c r="B29" s="180" t="s">
         <v>176</v>
       </c>
-      <c r="C29" s="243"/>
-      <c r="D29" s="244"/>
-      <c r="E29" s="239" t="s">
+      <c r="C29" s="296"/>
+      <c r="D29" s="297"/>
+      <c r="E29" s="292" t="s">
         <v>178</v>
       </c>
-      <c r="F29" s="239"/>
+      <c r="F29" s="292"/>
       <c r="G29" s="181"/>
     </row>
     <row r="30" spans="1:7" ht="14.25" customHeight="1" thickBot="1">
@@ -10219,12 +10237,12 @@
       <c r="B30" s="183" t="s">
         <v>177</v>
       </c>
-      <c r="C30" s="241"/>
-      <c r="D30" s="242"/>
-      <c r="E30" s="240" t="s">
+      <c r="C30" s="294"/>
+      <c r="D30" s="295"/>
+      <c r="E30" s="293" t="s">
         <v>167</v>
       </c>
-      <c r="F30" s="240"/>
+      <c r="F30" s="293"/>
       <c r="G30" s="184"/>
     </row>
     <row r="32" spans="1:7" ht="12.75" thickBot="1">
@@ -10239,20 +10257,32 @@
       <c r="B33" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="202" t="s">
+      <c r="C33" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="203"/>
-      <c r="E33" s="202" t="s">
+      <c r="D33" s="266"/>
+      <c r="E33" s="265" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="204"/>
+      <c r="F33" s="279"/>
       <c r="G33" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="C22:D22"/>
@@ -10265,18 +10295,6 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10286,8 +10304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10303,805 +10321,828 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="200" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="261"/>
-      <c r="C1" s="261"/>
-      <c r="D1" s="261"/>
-      <c r="E1" s="261"/>
-      <c r="F1" s="261"/>
-      <c r="G1" s="261"/>
-      <c r="H1" s="261"/>
-      <c r="I1" s="261"/>
-      <c r="J1" s="261"/>
-      <c r="K1" s="261"/>
-      <c r="L1" s="261"/>
-      <c r="M1" s="261"/>
-      <c r="N1" s="261"/>
-      <c r="O1" s="261"/>
-      <c r="P1" s="261"/>
-      <c r="Q1" s="261"/>
-      <c r="R1" s="261"/>
-      <c r="S1" s="261"/>
-      <c r="T1" s="261"/>
-      <c r="U1" s="261"/>
-      <c r="V1" s="261"/>
-    </row>
-    <row r="2" spans="1:22" ht="24">
-      <c r="A2" s="261"/>
-      <c r="B2" s="277" t="s">
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="199"/>
+      <c r="I1" s="199"/>
+      <c r="J1" s="199"/>
+      <c r="K1" s="199"/>
+      <c r="L1" s="199"/>
+      <c r="M1" s="199"/>
+      <c r="N1" s="199"/>
+      <c r="O1" s="199"/>
+      <c r="P1" s="199"/>
+      <c r="Q1" s="199"/>
+      <c r="R1" s="199"/>
+      <c r="S1" s="199"/>
+      <c r="T1" s="199"/>
+      <c r="U1" s="199"/>
+      <c r="V1" s="199"/>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="199"/>
+      <c r="B2" s="215" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="256" t="s">
         <v>193</v>
       </c>
-      <c r="D2" s="228"/>
-      <c r="E2" s="279" t="s">
+      <c r="D2" s="257"/>
+      <c r="E2" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="223" t="s">
+      <c r="F2" s="256" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="224"/>
-      <c r="H2" s="261"/>
-      <c r="I2" s="261"/>
-      <c r="J2" s="261"/>
-      <c r="K2" s="261"/>
-      <c r="L2" s="261"/>
-      <c r="M2" s="261"/>
-      <c r="N2" s="261"/>
-      <c r="O2" s="261"/>
-      <c r="P2" s="261"/>
-      <c r="Q2" s="261"/>
-      <c r="R2" s="261"/>
-      <c r="S2" s="261"/>
-      <c r="T2" s="261"/>
-      <c r="U2" s="261"/>
-      <c r="V2" s="261"/>
-    </row>
-    <row r="3" spans="1:22" ht="36">
-      <c r="A3" s="261"/>
-      <c r="B3" s="278" t="s">
+      <c r="G2" s="260"/>
+      <c r="H2" s="199"/>
+      <c r="I2" s="199"/>
+      <c r="J2" s="199"/>
+      <c r="K2" s="199"/>
+      <c r="L2" s="199"/>
+      <c r="M2" s="199"/>
+      <c r="N2" s="199"/>
+      <c r="O2" s="199"/>
+      <c r="P2" s="199"/>
+      <c r="Q2" s="199"/>
+      <c r="R2" s="199"/>
+      <c r="S2" s="199"/>
+      <c r="T2" s="199"/>
+      <c r="U2" s="199"/>
+      <c r="V2" s="199"/>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="199"/>
+      <c r="B3" s="216" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
-      <c r="E3" s="280" t="s">
+      <c r="C3" s="258"/>
+      <c r="D3" s="259"/>
+      <c r="E3" s="218" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="225" t="s">
+      <c r="F3" s="261" t="s">
         <v>192</v>
       </c>
-      <c r="G3" s="226"/>
-      <c r="H3" s="261"/>
-      <c r="I3" s="261"/>
-      <c r="J3" s="261"/>
-      <c r="K3" s="261"/>
-      <c r="L3" s="261"/>
-      <c r="M3" s="261"/>
-      <c r="N3" s="261"/>
-      <c r="O3" s="261"/>
-      <c r="P3" s="261"/>
-      <c r="Q3" s="261"/>
-      <c r="R3" s="261"/>
-      <c r="S3" s="261"/>
-      <c r="T3" s="261"/>
-      <c r="U3" s="261"/>
-      <c r="V3" s="261"/>
-    </row>
-    <row r="4" spans="1:22" ht="24">
-      <c r="A4" s="261"/>
-      <c r="B4" s="278" t="s">
+      <c r="G3" s="262"/>
+      <c r="H3" s="199"/>
+      <c r="I3" s="199"/>
+      <c r="J3" s="199"/>
+      <c r="K3" s="199"/>
+      <c r="L3" s="199"/>
+      <c r="M3" s="199"/>
+      <c r="N3" s="199"/>
+      <c r="O3" s="199"/>
+      <c r="P3" s="199"/>
+      <c r="Q3" s="199"/>
+      <c r="R3" s="199"/>
+      <c r="S3" s="199"/>
+      <c r="T3" s="199"/>
+      <c r="U3" s="199"/>
+      <c r="V3" s="199"/>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="199"/>
+      <c r="B4" s="216" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="227" t="s">
+      <c r="C4" s="258" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="229"/>
-      <c r="E4" s="280" t="s">
+      <c r="D4" s="259"/>
+      <c r="E4" s="218" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="226"/>
-      <c r="H4" s="261"/>
-      <c r="I4" s="261"/>
-      <c r="J4" s="261"/>
-      <c r="K4" s="261"/>
-      <c r="L4" s="261"/>
-      <c r="M4" s="261"/>
-      <c r="N4" s="261"/>
-      <c r="O4" s="261"/>
-      <c r="P4" s="261"/>
-      <c r="Q4" s="261"/>
-      <c r="R4" s="261"/>
-      <c r="S4" s="261"/>
-      <c r="T4" s="261"/>
-      <c r="U4" s="261"/>
-      <c r="V4" s="261"/>
-    </row>
-    <row r="5" spans="1:22" ht="36">
-      <c r="A5" s="261"/>
-      <c r="B5" s="278" t="s">
+      <c r="F4" s="258"/>
+      <c r="G4" s="262"/>
+      <c r="H4" s="199"/>
+      <c r="I4" s="199"/>
+      <c r="J4" s="199"/>
+      <c r="K4" s="199"/>
+      <c r="L4" s="199"/>
+      <c r="M4" s="199"/>
+      <c r="N4" s="199"/>
+      <c r="O4" s="199"/>
+      <c r="P4" s="199"/>
+      <c r="Q4" s="199"/>
+      <c r="R4" s="199"/>
+      <c r="S4" s="199"/>
+      <c r="T4" s="199"/>
+      <c r="U4" s="199"/>
+      <c r="V4" s="199"/>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="199"/>
+      <c r="B5" s="216" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="258" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="229"/>
-      <c r="E5" s="280"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="226"/>
-      <c r="H5" s="261"/>
-      <c r="I5" s="261"/>
-      <c r="J5" s="261"/>
-      <c r="K5" s="261"/>
-      <c r="L5" s="261"/>
-      <c r="M5" s="261"/>
-      <c r="N5" s="261"/>
-      <c r="O5" s="261"/>
-      <c r="P5" s="261"/>
-      <c r="Q5" s="261"/>
-      <c r="R5" s="261"/>
-      <c r="S5" s="261"/>
-      <c r="T5" s="261"/>
-      <c r="U5" s="261"/>
-      <c r="V5" s="261"/>
-    </row>
-    <row r="6" spans="1:22" ht="36">
-      <c r="A6" s="261"/>
-      <c r="B6" s="278" t="s">
+      <c r="D5" s="259"/>
+      <c r="E5" s="218"/>
+      <c r="F5" s="258"/>
+      <c r="G5" s="262"/>
+      <c r="H5" s="199"/>
+      <c r="I5" s="199"/>
+      <c r="J5" s="199"/>
+      <c r="K5" s="199"/>
+      <c r="L5" s="199"/>
+      <c r="M5" s="199"/>
+      <c r="N5" s="199"/>
+      <c r="O5" s="199"/>
+      <c r="P5" s="199"/>
+      <c r="Q5" s="199"/>
+      <c r="R5" s="199"/>
+      <c r="S5" s="199"/>
+      <c r="T5" s="199"/>
+      <c r="U5" s="199"/>
+      <c r="V5" s="199"/>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="199"/>
+      <c r="B6" s="216" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="258" t="s">
         <v>181</v>
       </c>
-      <c r="D6" s="229"/>
-      <c r="E6" s="281"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="226"/>
-      <c r="H6" s="261"/>
-      <c r="I6" s="261"/>
-      <c r="J6" s="261"/>
-      <c r="K6" s="261"/>
-      <c r="L6" s="261"/>
-      <c r="M6" s="261"/>
-      <c r="N6" s="261"/>
-      <c r="O6" s="261"/>
-      <c r="P6" s="261"/>
-      <c r="Q6" s="261"/>
-      <c r="R6" s="261"/>
-      <c r="S6" s="261"/>
-      <c r="T6" s="261"/>
-      <c r="U6" s="261"/>
-      <c r="V6" s="261"/>
+      <c r="D6" s="259"/>
+      <c r="E6" s="219"/>
+      <c r="F6" s="258"/>
+      <c r="G6" s="262"/>
+      <c r="H6" s="199"/>
+      <c r="I6" s="199"/>
+      <c r="J6" s="199"/>
+      <c r="K6" s="199"/>
+      <c r="L6" s="199"/>
+      <c r="M6" s="199"/>
+      <c r="N6" s="199"/>
+      <c r="O6" s="199"/>
+      <c r="P6" s="199"/>
+      <c r="Q6" s="199"/>
+      <c r="R6" s="199"/>
+      <c r="S6" s="199"/>
+      <c r="T6" s="199"/>
+      <c r="U6" s="199"/>
+      <c r="V6" s="199"/>
     </row>
     <row r="7" spans="1:22">
-      <c r="A7" s="261"/>
-      <c r="B7" s="211" t="s">
+      <c r="A7" s="199"/>
+      <c r="B7" s="267" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="212"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="213"/>
-      <c r="H7" s="261"/>
-      <c r="I7" s="261"/>
-      <c r="J7" s="261"/>
-      <c r="K7" s="261"/>
-      <c r="L7" s="261"/>
-      <c r="M7" s="261"/>
-      <c r="N7" s="261"/>
-      <c r="O7" s="261"/>
-      <c r="P7" s="261"/>
-      <c r="Q7" s="261"/>
-      <c r="R7" s="261"/>
-      <c r="S7" s="261"/>
-      <c r="T7" s="261"/>
-      <c r="U7" s="261"/>
-      <c r="V7" s="261"/>
+      <c r="C7" s="268"/>
+      <c r="D7" s="268"/>
+      <c r="E7" s="268"/>
+      <c r="F7" s="268"/>
+      <c r="G7" s="269"/>
+      <c r="H7" s="199"/>
+      <c r="I7" s="199"/>
+      <c r="J7" s="199"/>
+      <c r="K7" s="199"/>
+      <c r="L7" s="199"/>
+      <c r="M7" s="199"/>
+      <c r="N7" s="199"/>
+      <c r="O7" s="199"/>
+      <c r="P7" s="199"/>
+      <c r="Q7" s="199"/>
+      <c r="R7" s="199"/>
+      <c r="S7" s="199"/>
+      <c r="T7" s="199"/>
+      <c r="U7" s="199"/>
+      <c r="V7" s="199"/>
     </row>
     <row r="8" spans="1:22">
-      <c r="A8" s="261"/>
-      <c r="B8" s="214"/>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
-      <c r="H8" s="261"/>
-      <c r="I8" s="261"/>
-      <c r="J8" s="261"/>
-      <c r="K8" s="261"/>
-      <c r="L8" s="261"/>
-      <c r="M8" s="261"/>
-      <c r="N8" s="261"/>
-      <c r="O8" s="261"/>
-      <c r="P8" s="261"/>
-      <c r="Q8" s="261"/>
-      <c r="R8" s="261"/>
-      <c r="S8" s="261"/>
-      <c r="T8" s="261"/>
-      <c r="U8" s="261"/>
-      <c r="V8" s="261"/>
+      <c r="A8" s="199"/>
+      <c r="B8" s="270"/>
+      <c r="C8" s="271"/>
+      <c r="D8" s="271"/>
+      <c r="E8" s="271"/>
+      <c r="F8" s="271"/>
+      <c r="G8" s="272"/>
+      <c r="H8" s="199"/>
+      <c r="I8" s="199"/>
+      <c r="J8" s="199"/>
+      <c r="K8" s="199"/>
+      <c r="L8" s="199"/>
+      <c r="M8" s="199"/>
+      <c r="N8" s="199"/>
+      <c r="O8" s="199"/>
+      <c r="P8" s="199"/>
+      <c r="Q8" s="199"/>
+      <c r="R8" s="199"/>
+      <c r="S8" s="199"/>
+      <c r="T8" s="199"/>
+      <c r="U8" s="199"/>
+      <c r="V8" s="199"/>
     </row>
     <row r="9" spans="1:22">
-      <c r="A9" s="261"/>
-      <c r="B9" s="217"/>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="216"/>
-      <c r="H9" s="261"/>
-      <c r="I9" s="261"/>
-      <c r="J9" s="261"/>
-      <c r="K9" s="261"/>
-      <c r="L9" s="261"/>
-      <c r="M9" s="261"/>
-      <c r="N9" s="261"/>
-      <c r="O9" s="261"/>
-      <c r="P9" s="261"/>
-      <c r="Q9" s="261"/>
-      <c r="R9" s="261"/>
-      <c r="S9" s="261"/>
-      <c r="T9" s="261"/>
-      <c r="U9" s="261"/>
-      <c r="V9" s="261"/>
+      <c r="A9" s="199"/>
+      <c r="B9" s="273"/>
+      <c r="C9" s="271"/>
+      <c r="D9" s="271"/>
+      <c r="E9" s="271"/>
+      <c r="F9" s="271"/>
+      <c r="G9" s="272"/>
+      <c r="H9" s="199"/>
+      <c r="I9" s="199"/>
+      <c r="J9" s="199"/>
+      <c r="K9" s="199"/>
+      <c r="L9" s="199"/>
+      <c r="M9" s="199"/>
+      <c r="N9" s="199"/>
+      <c r="O9" s="199"/>
+      <c r="P9" s="199"/>
+      <c r="Q9" s="199"/>
+      <c r="R9" s="199"/>
+      <c r="S9" s="199"/>
+      <c r="T9" s="199"/>
+      <c r="U9" s="199"/>
+      <c r="V9" s="199"/>
     </row>
     <row r="10" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A10" s="261"/>
-      <c r="B10" s="218"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="220"/>
-      <c r="H10" s="261"/>
-      <c r="I10" s="261"/>
-      <c r="J10" s="261"/>
-      <c r="K10" s="261"/>
-      <c r="L10" s="261"/>
-      <c r="M10" s="261"/>
-      <c r="N10" s="261"/>
-      <c r="O10" s="261"/>
-      <c r="P10" s="261"/>
-      <c r="Q10" s="261"/>
-      <c r="R10" s="261"/>
-      <c r="S10" s="261"/>
-      <c r="T10" s="261"/>
-      <c r="U10" s="261"/>
-      <c r="V10" s="261"/>
+      <c r="A10" s="199"/>
+      <c r="B10" s="274"/>
+      <c r="C10" s="275"/>
+      <c r="D10" s="275"/>
+      <c r="E10" s="275"/>
+      <c r="F10" s="275"/>
+      <c r="G10" s="276"/>
+      <c r="H10" s="199"/>
+      <c r="I10" s="199"/>
+      <c r="J10" s="199"/>
+      <c r="K10" s="199"/>
+      <c r="L10" s="199"/>
+      <c r="M10" s="199"/>
+      <c r="N10" s="199"/>
+      <c r="O10" s="199"/>
+      <c r="P10" s="199"/>
+      <c r="Q10" s="199"/>
+      <c r="R10" s="199"/>
+      <c r="S10" s="199"/>
+      <c r="T10" s="199"/>
+      <c r="U10" s="199"/>
+      <c r="V10" s="199"/>
     </row>
     <row r="12" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A12" s="262" t="s">
+      <c r="A12" s="200" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="261"/>
-      <c r="C12" s="261"/>
-      <c r="D12" s="261"/>
-      <c r="E12" s="261"/>
-      <c r="F12" s="261"/>
-      <c r="G12" s="261"/>
-      <c r="H12" s="261"/>
-      <c r="I12" s="261"/>
-      <c r="J12" s="261"/>
-      <c r="K12" s="261"/>
-      <c r="L12" s="261"/>
-      <c r="M12" s="261"/>
-      <c r="N12" s="261"/>
-      <c r="O12" s="261"/>
-      <c r="P12" s="261"/>
-      <c r="Q12" s="261"/>
-      <c r="R12" s="261"/>
-      <c r="S12" s="261"/>
-      <c r="T12" s="261"/>
-      <c r="U12" s="261"/>
-      <c r="V12" s="261"/>
+      <c r="B12" s="199"/>
+      <c r="C12" s="199"/>
+      <c r="D12" s="199"/>
+      <c r="E12" s="199"/>
+      <c r="F12" s="199"/>
+      <c r="G12" s="199"/>
+      <c r="H12" s="199"/>
+      <c r="I12" s="199"/>
+      <c r="J12" s="199"/>
+      <c r="K12" s="199"/>
+      <c r="L12" s="199"/>
+      <c r="M12" s="199"/>
+      <c r="N12" s="199"/>
+      <c r="O12" s="199"/>
+      <c r="P12" s="199"/>
+      <c r="Q12" s="199"/>
+      <c r="R12" s="199"/>
+      <c r="S12" s="199"/>
+      <c r="T12" s="199"/>
+      <c r="U12" s="199"/>
+      <c r="V12" s="199"/>
     </row>
     <row r="13" spans="1:22" ht="24">
-      <c r="A13" s="268" t="s">
+      <c r="A13" s="206" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="269" t="s">
+      <c r="B13" s="207" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="269" t="s">
+      <c r="C13" s="207" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="269" t="s">
+      <c r="D13" s="207" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="270" t="s">
+      <c r="E13" s="208" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="269" t="s">
+      <c r="F13" s="207" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="271" t="s">
+      <c r="G13" s="209" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="310"/>
-      <c r="M13" s="315"/>
-      <c r="N13" s="315"/>
-      <c r="O13" s="315"/>
-      <c r="P13" s="299"/>
-      <c r="Q13" s="299"/>
-      <c r="R13" s="299"/>
-      <c r="S13" s="299"/>
-      <c r="T13" s="299"/>
-      <c r="U13" s="299"/>
-      <c r="V13" s="299"/>
+      <c r="H13" s="245"/>
+      <c r="M13" s="249"/>
+      <c r="N13" s="249"/>
+      <c r="O13" s="249"/>
+      <c r="P13" s="236"/>
+      <c r="Q13" s="236"/>
+      <c r="R13" s="236"/>
+      <c r="S13" s="236"/>
+      <c r="T13" s="236"/>
+      <c r="U13" s="236"/>
+      <c r="V13" s="236"/>
     </row>
     <row r="14" spans="1:22">
-      <c r="A14" s="287">
+      <c r="A14" s="315">
+        <v>1</v>
+      </c>
+      <c r="B14" s="316" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" s="317" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" s="318" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" s="319" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="320"/>
+      <c r="G14" s="321"/>
+      <c r="H14" s="314"/>
+      <c r="M14" s="237"/>
+      <c r="N14" s="237"/>
+      <c r="O14" s="236"/>
+      <c r="P14" s="236"/>
+      <c r="Q14" s="236"/>
+      <c r="R14" s="236"/>
+      <c r="S14" s="236"/>
+      <c r="T14" s="236"/>
+      <c r="U14" s="236"/>
+      <c r="V14" s="236"/>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A15" s="225">
         <v>2</v>
       </c>
-      <c r="B14" s="288" t="s">
-        <v>186</v>
-      </c>
-      <c r="C14" s="289" t="s">
+      <c r="B15" s="226" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="227" t="s">
+        <v>189</v>
+      </c>
+      <c r="D15" s="227" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" s="228" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="229"/>
+      <c r="G15" s="233"/>
+      <c r="H15" s="236"/>
+      <c r="I15" s="236"/>
+      <c r="J15" s="236"/>
+      <c r="K15" s="236"/>
+      <c r="L15" s="236"/>
+      <c r="M15" s="236"/>
+      <c r="N15" s="236"/>
+      <c r="O15" s="236"/>
+      <c r="P15" s="236"/>
+      <c r="Q15" s="236"/>
+      <c r="R15" s="236"/>
+      <c r="S15" s="236"/>
+      <c r="T15" s="236"/>
+      <c r="U15" s="236"/>
+      <c r="V15" s="236"/>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="225">
+        <v>3</v>
+      </c>
+      <c r="B16" s="226" t="s">
+        <v>190</v>
+      </c>
+      <c r="C16" s="241" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16" s="234" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" s="228" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="229"/>
+      <c r="G16" s="232"/>
+      <c r="H16" s="236"/>
+      <c r="I16" s="246" t="s">
         <v>182</v>
       </c>
-      <c r="D14" s="177" t="s">
-        <v>155</v>
-      </c>
-      <c r="E14" s="290" t="s">
+      <c r="J16" s="246" t="s">
+        <v>140</v>
+      </c>
+      <c r="K16" s="246" t="s">
+        <v>183</v>
+      </c>
+      <c r="L16" s="242" t="s">
+        <v>184</v>
+      </c>
+      <c r="M16" s="236"/>
+      <c r="N16" s="236"/>
+      <c r="O16" s="236"/>
+      <c r="P16" s="236"/>
+      <c r="Q16" s="236"/>
+      <c r="R16" s="236"/>
+      <c r="S16" s="236"/>
+      <c r="T16" s="236"/>
+      <c r="U16" s="236"/>
+      <c r="V16" s="236"/>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17" s="225">
+        <v>4</v>
+      </c>
+      <c r="B17" s="226" t="s">
+        <v>191</v>
+      </c>
+      <c r="C17" s="227" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="177" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="228" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="291"/>
-      <c r="G14" s="295"/>
-      <c r="H14" s="314"/>
-      <c r="M14" s="300"/>
-      <c r="N14" s="300"/>
-      <c r="O14" s="299"/>
-      <c r="P14" s="299"/>
-      <c r="Q14" s="299"/>
-      <c r="R14" s="299"/>
-      <c r="S14" s="299"/>
-      <c r="T14" s="299"/>
-      <c r="U14" s="299"/>
-      <c r="V14" s="299"/>
-    </row>
-    <row r="15" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A15" s="287">
+      <c r="F17" s="229"/>
+      <c r="G17" s="232"/>
+      <c r="H17" s="236"/>
+      <c r="I17" s="243" t="s">
+        <v>185</v>
+      </c>
+      <c r="J17" s="247">
+        <v>40901</v>
+      </c>
+      <c r="K17" s="247">
+        <v>40902</v>
+      </c>
+      <c r="L17" s="250">
+        <v>1</v>
+      </c>
+      <c r="M17" s="236"/>
+      <c r="N17" s="236"/>
+      <c r="O17" s="236"/>
+      <c r="P17" s="236"/>
+      <c r="Q17" s="236"/>
+      <c r="R17" s="236"/>
+      <c r="S17" s="236"/>
+      <c r="T17" s="236"/>
+      <c r="U17" s="236"/>
+      <c r="V17" s="236"/>
+    </row>
+    <row r="18" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A18" s="231">
+        <v>5</v>
+      </c>
+      <c r="B18" s="238" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="230" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="158" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="239" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="288" t="s">
-        <v>145</v>
-      </c>
-      <c r="C15" s="289" t="s">
-        <v>189</v>
-      </c>
-      <c r="D15" s="289" t="s">
-        <v>152</v>
-      </c>
-      <c r="E15" s="290"/>
-      <c r="F15" s="291"/>
-      <c r="G15" s="296"/>
-      <c r="H15" s="310"/>
-      <c r="I15" s="299"/>
-      <c r="J15" s="299"/>
-      <c r="K15" s="299"/>
-      <c r="L15" s="299"/>
-      <c r="M15" s="299"/>
-      <c r="N15" s="299"/>
-      <c r="O15" s="299"/>
-      <c r="P15" s="299"/>
-      <c r="Q15" s="299"/>
-      <c r="R15" s="299"/>
-      <c r="S15" s="299"/>
-      <c r="T15" s="299"/>
-      <c r="U15" s="299"/>
-      <c r="V15" s="299"/>
-    </row>
-    <row r="16" spans="1:22">
-      <c r="A16" s="287">
-        <v>4</v>
-      </c>
-      <c r="B16" s="288" t="s">
-        <v>190</v>
-      </c>
-      <c r="C16" s="306" t="s">
-        <v>183</v>
-      </c>
-      <c r="D16" s="297" t="s">
-        <v>152</v>
-      </c>
-      <c r="E16" s="290"/>
-      <c r="F16" s="291"/>
-      <c r="G16" s="294"/>
-      <c r="H16" s="310"/>
-      <c r="I16" s="311" t="s">
-        <v>182</v>
-      </c>
-      <c r="J16" s="311" t="s">
-        <v>140</v>
-      </c>
-      <c r="K16" s="311" t="s">
-        <v>183</v>
-      </c>
-      <c r="L16" s="307" t="s">
-        <v>184</v>
-      </c>
-      <c r="M16" s="299"/>
-      <c r="N16" s="299"/>
-      <c r="O16" s="299"/>
-      <c r="P16" s="299"/>
-      <c r="Q16" s="299"/>
-      <c r="R16" s="299"/>
-      <c r="S16" s="299"/>
-      <c r="T16" s="299"/>
-      <c r="U16" s="299"/>
-      <c r="V16" s="299"/>
-    </row>
-    <row r="17" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A17" s="293">
+      <c r="F18" s="322"/>
+      <c r="G18" s="323"/>
+      <c r="I18" s="244" t="s">
+        <v>187</v>
+      </c>
+      <c r="J18" s="244" t="s">
+        <v>188</v>
+      </c>
+      <c r="K18" s="248">
+        <v>40493</v>
+      </c>
+      <c r="L18" s="251">
+        <v>41255</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A19" s="200" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="199"/>
+      <c r="C19" s="199"/>
+      <c r="D19" s="199"/>
+      <c r="E19" s="199"/>
+      <c r="F19" s="199"/>
+      <c r="G19" s="199"/>
+      <c r="H19" s="199"/>
+      <c r="I19" s="199"/>
+      <c r="J19" s="199"/>
+      <c r="K19" s="199"/>
+      <c r="L19" s="199"/>
+      <c r="M19" s="199"/>
+      <c r="N19" s="199"/>
+      <c r="O19" s="199"/>
+      <c r="P19" s="199"/>
+      <c r="Q19" s="199"/>
+      <c r="R19" s="199"/>
+      <c r="S19" s="199"/>
+      <c r="T19" s="199"/>
+      <c r="U19" s="199"/>
+      <c r="V19" s="199"/>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20" s="205" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="210" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="263" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="264"/>
+      <c r="E20" s="210" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="210" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="211" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="199"/>
+      <c r="I20" s="199"/>
+      <c r="J20" s="199"/>
+      <c r="K20" s="199"/>
+      <c r="L20" s="199"/>
+      <c r="M20" s="199"/>
+      <c r="N20" s="199"/>
+      <c r="O20" s="199"/>
+      <c r="P20" s="199"/>
+      <c r="Q20" s="199"/>
+      <c r="R20" s="199"/>
+      <c r="S20" s="199"/>
+      <c r="T20" s="199"/>
+      <c r="U20" s="199"/>
+      <c r="V20" s="199"/>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21" s="202">
+        <v>1</v>
+      </c>
+      <c r="B21" s="203" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="301" t="s">
-        <v>191</v>
-      </c>
-      <c r="C17" s="292" t="s">
+      <c r="C21" s="302" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" s="303"/>
+      <c r="E21" s="220" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="220" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="204"/>
+      <c r="H21" s="199"/>
+      <c r="I21" s="199"/>
+      <c r="J21" s="199"/>
+      <c r="K21" s="199"/>
+      <c r="L21" s="199"/>
+      <c r="M21" s="199"/>
+      <c r="N21" s="199"/>
+      <c r="O21" s="199"/>
+      <c r="P21" s="199"/>
+      <c r="Q21" s="199"/>
+      <c r="R21" s="199"/>
+      <c r="S21" s="199"/>
+      <c r="T21" s="199"/>
+      <c r="U21" s="199"/>
+      <c r="V21" s="199"/>
+    </row>
+    <row r="22" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A22" s="223">
+        <v>2</v>
+      </c>
+      <c r="B22" s="221" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22" s="304" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="305"/>
+      <c r="E22" s="224"/>
+      <c r="F22" s="224"/>
+      <c r="G22" s="222"/>
+      <c r="H22" s="199"/>
+      <c r="I22" s="199"/>
+      <c r="J22" s="199"/>
+      <c r="K22" s="199"/>
+      <c r="L22" s="199"/>
+      <c r="M22" s="199"/>
+      <c r="N22" s="199"/>
+      <c r="O22" s="199"/>
+      <c r="P22" s="199"/>
+      <c r="Q22" s="199"/>
+      <c r="R22" s="199"/>
+      <c r="S22" s="199"/>
+      <c r="T22" s="199"/>
+      <c r="U22" s="199"/>
+      <c r="V22" s="199"/>
+    </row>
+    <row r="24" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A24" s="200" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="199"/>
+      <c r="C24" s="199"/>
+      <c r="D24" s="199"/>
+      <c r="E24" s="199"/>
+      <c r="F24" s="199"/>
+      <c r="G24" s="199"/>
+      <c r="H24" s="199"/>
+      <c r="I24" s="199"/>
+      <c r="J24" s="199"/>
+      <c r="K24" s="199"/>
+      <c r="L24" s="199"/>
+      <c r="M24" s="199"/>
+      <c r="N24" s="199"/>
+      <c r="O24" s="199"/>
+      <c r="P24" s="199"/>
+      <c r="Q24" s="199"/>
+      <c r="R24" s="199"/>
+      <c r="S24" s="199"/>
+      <c r="T24" s="199"/>
+      <c r="U24" s="199"/>
+      <c r="V24" s="199"/>
+    </row>
+    <row r="25" spans="1:22" ht="24.75" thickBot="1">
+      <c r="A25" s="212" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="213" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="265" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="266"/>
+      <c r="E25" s="265" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="279"/>
+      <c r="G25" s="214" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="199"/>
+      <c r="I25" s="199"/>
+      <c r="J25" s="199"/>
+      <c r="K25" s="199"/>
+      <c r="L25" s="199"/>
+      <c r="M25" s="199"/>
+      <c r="N25" s="199"/>
+      <c r="O25" s="199"/>
+      <c r="P25" s="199"/>
+      <c r="Q25" s="199"/>
+      <c r="R25" s="199"/>
+      <c r="S25" s="199"/>
+      <c r="T25" s="199"/>
+      <c r="U25" s="199"/>
+      <c r="V25" s="199"/>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="A26" s="201">
+        <v>1</v>
+      </c>
+      <c r="B26" s="198" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="300" t="s">
         <v>159</v>
       </c>
-      <c r="D17" s="158" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="302"/>
-      <c r="F17" s="303"/>
-      <c r="G17" s="304"/>
-      <c r="H17" s="310"/>
-      <c r="I17" s="308" t="s">
-        <v>185</v>
-      </c>
-      <c r="J17" s="312">
-        <v>40901</v>
-      </c>
-      <c r="K17" s="312">
-        <v>40902</v>
-      </c>
-      <c r="L17" s="316">
-        <v>1</v>
-      </c>
-      <c r="M17" s="299"/>
-      <c r="N17" s="299"/>
-      <c r="O17" s="299"/>
-      <c r="P17" s="299"/>
-      <c r="Q17" s="299"/>
-      <c r="R17" s="299"/>
-      <c r="S17" s="299"/>
-      <c r="T17" s="299"/>
-      <c r="U17" s="299"/>
-      <c r="V17" s="299"/>
-    </row>
-    <row r="18" spans="1:22" ht="15.75" thickBot="1">
-      <c r="I18" s="309" t="s">
-        <v>187</v>
-      </c>
-      <c r="J18" s="309" t="s">
-        <v>188</v>
-      </c>
-      <c r="K18" s="313">
-        <v>40493</v>
-      </c>
-      <c r="L18" s="317">
-        <v>41255</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A19" s="262" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="261"/>
-      <c r="C19" s="261"/>
-      <c r="D19" s="261"/>
-      <c r="E19" s="261"/>
-      <c r="F19" s="261"/>
-      <c r="G19" s="261"/>
-      <c r="H19" s="261"/>
-      <c r="I19" s="261"/>
-      <c r="J19" s="261"/>
-      <c r="K19" s="261"/>
-      <c r="L19" s="261"/>
-      <c r="M19" s="261"/>
-      <c r="N19" s="261"/>
-      <c r="O19" s="261"/>
-      <c r="P19" s="261"/>
-      <c r="Q19" s="261"/>
-      <c r="R19" s="261"/>
-      <c r="S19" s="261"/>
-      <c r="T19" s="261"/>
-      <c r="U19" s="261"/>
-      <c r="V19" s="261"/>
-    </row>
-    <row r="20" spans="1:22">
-      <c r="A20" s="267" t="s">
+      <c r="D26" s="301"/>
+      <c r="E26" s="299" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="299"/>
+      <c r="G26" s="235" t="s">
+        <v>114</v>
+      </c>
+      <c r="H26" s="199"/>
+      <c r="I26" s="199"/>
+      <c r="J26" s="199"/>
+      <c r="K26" s="199"/>
+      <c r="L26" s="199"/>
+      <c r="M26" s="199"/>
+      <c r="N26" s="199"/>
+      <c r="O26" s="199"/>
+      <c r="P26" s="199"/>
+      <c r="Q26" s="199"/>
+      <c r="R26" s="199"/>
+      <c r="S26" s="199"/>
+      <c r="T26" s="199"/>
+      <c r="U26" s="199"/>
+      <c r="V26" s="199"/>
+    </row>
+    <row r="27" spans="1:22">
+      <c r="A27" s="199"/>
+      <c r="B27" s="199"/>
+      <c r="C27" s="240"/>
+      <c r="D27" s="240"/>
+      <c r="E27" s="240"/>
+      <c r="F27" s="240"/>
+      <c r="G27" s="199"/>
+      <c r="H27" s="199"/>
+      <c r="I27" s="199"/>
+      <c r="J27" s="199"/>
+      <c r="K27" s="199"/>
+      <c r="L27" s="199"/>
+      <c r="M27" s="199"/>
+      <c r="N27" s="199"/>
+      <c r="O27" s="199"/>
+      <c r="P27" s="199"/>
+      <c r="Q27" s="199"/>
+      <c r="R27" s="199"/>
+      <c r="S27" s="199"/>
+      <c r="T27" s="199"/>
+      <c r="U27" s="199"/>
+      <c r="V27" s="199"/>
+    </row>
+    <row r="28" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A28" s="200" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="199"/>
+      <c r="C28" s="199"/>
+      <c r="D28" s="199"/>
+      <c r="E28" s="199"/>
+      <c r="F28" s="199"/>
+      <c r="G28" s="199"/>
+      <c r="H28" s="199"/>
+      <c r="I28" s="199"/>
+      <c r="J28" s="199"/>
+      <c r="K28" s="199"/>
+      <c r="L28" s="199"/>
+      <c r="M28" s="199"/>
+      <c r="N28" s="199"/>
+      <c r="O28" s="199"/>
+      <c r="P28" s="199"/>
+      <c r="Q28" s="199"/>
+      <c r="R28" s="199"/>
+      <c r="S28" s="199"/>
+      <c r="T28" s="199"/>
+      <c r="U28" s="199"/>
+      <c r="V28" s="199"/>
+    </row>
+    <row r="29" spans="1:22" ht="24.75" thickBot="1">
+      <c r="A29" s="212" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="272" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="209" t="s">
+      <c r="B29" s="213" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="210"/>
-      <c r="E20" s="272" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="272" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="273" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="261"/>
-      <c r="I20" s="261"/>
-      <c r="J20" s="261"/>
-      <c r="K20" s="261"/>
-      <c r="L20" s="261"/>
-      <c r="M20" s="261"/>
-      <c r="N20" s="261"/>
-      <c r="O20" s="261"/>
-      <c r="P20" s="261"/>
-      <c r="Q20" s="261"/>
-      <c r="R20" s="261"/>
-      <c r="S20" s="261"/>
-      <c r="T20" s="261"/>
-      <c r="U20" s="261"/>
-      <c r="V20" s="261"/>
-    </row>
-    <row r="21" spans="1:22">
-      <c r="A21" s="264">
-        <v>1</v>
-      </c>
-      <c r="B21" s="265" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="249" t="s">
-        <v>194</v>
-      </c>
-      <c r="D21" s="250"/>
-      <c r="E21" s="282" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="282" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="266"/>
-      <c r="H21" s="261"/>
-      <c r="I21" s="261"/>
-      <c r="J21" s="261"/>
-      <c r="K21" s="261"/>
-      <c r="L21" s="261"/>
-      <c r="M21" s="261"/>
-      <c r="N21" s="261"/>
-      <c r="O21" s="261"/>
-      <c r="P21" s="261"/>
-      <c r="Q21" s="261"/>
-      <c r="R21" s="261"/>
-      <c r="S21" s="261"/>
-      <c r="T21" s="261"/>
-      <c r="U21" s="261"/>
-      <c r="V21" s="261"/>
-    </row>
-    <row r="22" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A22" s="285">
-        <v>2</v>
-      </c>
-      <c r="B22" s="283" t="s">
-        <v>195</v>
-      </c>
-      <c r="C22" s="247" t="s">
-        <v>171</v>
-      </c>
-      <c r="D22" s="248"/>
-      <c r="E22" s="286"/>
-      <c r="F22" s="286"/>
-      <c r="G22" s="284"/>
-      <c r="H22" s="261"/>
-      <c r="I22" s="261"/>
-      <c r="J22" s="261"/>
-      <c r="K22" s="261"/>
-      <c r="L22" s="261"/>
-      <c r="M22" s="261"/>
-      <c r="N22" s="261"/>
-      <c r="O22" s="261"/>
-      <c r="P22" s="261"/>
-      <c r="Q22" s="261"/>
-      <c r="R22" s="261"/>
-      <c r="S22" s="261"/>
-      <c r="T22" s="261"/>
-      <c r="U22" s="261"/>
-      <c r="V22" s="261"/>
-    </row>
-    <row r="24" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A24" s="262" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="261"/>
-      <c r="C24" s="261"/>
-      <c r="D24" s="261"/>
-      <c r="E24" s="261"/>
-      <c r="F24" s="261"/>
-      <c r="G24" s="261"/>
-      <c r="H24" s="261"/>
-      <c r="I24" s="261"/>
-      <c r="J24" s="261"/>
-      <c r="K24" s="261"/>
-      <c r="L24" s="261"/>
-      <c r="M24" s="261"/>
-      <c r="N24" s="261"/>
-      <c r="O24" s="261"/>
-      <c r="P24" s="261"/>
-      <c r="Q24" s="261"/>
-      <c r="R24" s="261"/>
-      <c r="S24" s="261"/>
-      <c r="T24" s="261"/>
-      <c r="U24" s="261"/>
-      <c r="V24" s="261"/>
-    </row>
-    <row r="25" spans="1:22" ht="24.75" thickBot="1">
-      <c r="A25" s="274" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="275" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="202" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="203"/>
-      <c r="E25" s="202" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="204"/>
-      <c r="G25" s="276" t="s">
-        <v>38</v>
-      </c>
-      <c r="H25" s="261"/>
-      <c r="I25" s="261"/>
-      <c r="J25" s="261"/>
-      <c r="K25" s="261"/>
-      <c r="L25" s="261"/>
-      <c r="M25" s="261"/>
-      <c r="N25" s="261"/>
-      <c r="O25" s="261"/>
-      <c r="P25" s="261"/>
-      <c r="Q25" s="261"/>
-      <c r="R25" s="261"/>
-      <c r="S25" s="261"/>
-      <c r="T25" s="261"/>
-      <c r="U25" s="261"/>
-      <c r="V25" s="261"/>
-    </row>
-    <row r="26" spans="1:22">
-      <c r="A26" s="263">
-        <v>1</v>
-      </c>
-      <c r="B26" s="258" t="s">
-        <v>196</v>
-      </c>
-      <c r="C26" s="257" t="s">
-        <v>159</v>
-      </c>
-      <c r="D26" s="259"/>
-      <c r="E26" s="260" t="s">
-        <v>129</v>
-      </c>
-      <c r="F26" s="260"/>
-      <c r="G26" s="298" t="s">
-        <v>114</v>
-      </c>
-      <c r="H26" s="261"/>
-      <c r="I26" s="261"/>
-      <c r="J26" s="261"/>
-      <c r="K26" s="261"/>
-      <c r="L26" s="261"/>
-      <c r="M26" s="261"/>
-      <c r="N26" s="261"/>
-      <c r="O26" s="261"/>
-      <c r="P26" s="261"/>
-      <c r="Q26" s="261"/>
-      <c r="R26" s="261"/>
-      <c r="S26" s="261"/>
-      <c r="T26" s="261"/>
-      <c r="U26" s="261"/>
-      <c r="V26" s="261"/>
-    </row>
-    <row r="27" spans="1:22">
-      <c r="A27" s="261"/>
-      <c r="B27" s="261"/>
-      <c r="C27" s="305"/>
-      <c r="D27" s="305"/>
-      <c r="E27" s="305"/>
-      <c r="F27" s="305"/>
-      <c r="G27" s="261"/>
-      <c r="H27" s="261"/>
-      <c r="I27" s="261"/>
-      <c r="J27" s="261"/>
-      <c r="K27" s="261"/>
-      <c r="L27" s="261"/>
-      <c r="M27" s="261"/>
-      <c r="N27" s="261"/>
-      <c r="O27" s="261"/>
-      <c r="P27" s="261"/>
-      <c r="Q27" s="261"/>
-      <c r="R27" s="261"/>
-      <c r="S27" s="261"/>
-      <c r="T27" s="261"/>
-      <c r="U27" s="261"/>
-      <c r="V27" s="261"/>
-    </row>
-    <row r="28" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A28" s="262" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="261"/>
-      <c r="C28" s="261"/>
-      <c r="D28" s="261"/>
-      <c r="E28" s="261"/>
-      <c r="F28" s="261"/>
-      <c r="G28" s="261"/>
-      <c r="H28" s="261"/>
-      <c r="I28" s="261"/>
-      <c r="J28" s="261"/>
-      <c r="K28" s="261"/>
-      <c r="L28" s="261"/>
-      <c r="M28" s="261"/>
-      <c r="N28" s="261"/>
-      <c r="O28" s="261"/>
-      <c r="P28" s="261"/>
-      <c r="Q28" s="261"/>
-      <c r="R28" s="261"/>
-      <c r="S28" s="261"/>
-      <c r="T28" s="261"/>
-      <c r="U28" s="261"/>
-      <c r="V28" s="261"/>
-    </row>
-    <row r="29" spans="1:22" ht="48.75" thickBot="1">
-      <c r="A29" s="274" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="275" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="202" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" s="203"/>
-      <c r="E29" s="202" t="s">
+      <c r="D29" s="266"/>
+      <c r="E29" s="265" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="204"/>
-      <c r="G29" s="276" t="s">
+      <c r="F29" s="279"/>
+      <c r="G29" s="214" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C25:D25"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E25:F25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11139,103 +11180,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="256" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="228"/>
+      <c r="D2" s="257"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="223" t="s">
+      <c r="F2" s="256" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="224"/>
+      <c r="G2" s="260"/>
     </row>
     <row r="3" spans="1:11" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
+      <c r="C3" s="258"/>
+      <c r="D3" s="259"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="227" t="s">
+      <c r="F3" s="258" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="226"/>
+      <c r="G3" s="262"/>
     </row>
     <row r="4" spans="1:11" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="227" t="s">
+      <c r="C4" s="258" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="229"/>
+      <c r="D4" s="259"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="226"/>
+      <c r="F4" s="258"/>
+      <c r="G4" s="262"/>
     </row>
     <row r="5" spans="1:11" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="258" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="229"/>
+      <c r="D5" s="259"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="226"/>
+      <c r="F5" s="258"/>
+      <c r="G5" s="262"/>
     </row>
     <row r="6" spans="1:11" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="258" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="229"/>
+      <c r="D6" s="259"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="226"/>
+      <c r="F6" s="258"/>
+      <c r="G6" s="262"/>
     </row>
     <row r="7" spans="1:11" ht="14.25">
-      <c r="B7" s="211" t="s">
+      <c r="B7" s="267" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="212"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="213"/>
+      <c r="C7" s="268"/>
+      <c r="D7" s="268"/>
+      <c r="E7" s="268"/>
+      <c r="F7" s="268"/>
+      <c r="G7" s="269"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="B8" s="214"/>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
+      <c r="B8" s="270"/>
+      <c r="C8" s="271"/>
+      <c r="D8" s="271"/>
+      <c r="E8" s="271"/>
+      <c r="F8" s="271"/>
+      <c r="G8" s="272"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9" s="217"/>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="216"/>
+      <c r="B9" s="273"/>
+      <c r="C9" s="271"/>
+      <c r="D9" s="271"/>
+      <c r="E9" s="271"/>
+      <c r="F9" s="271"/>
+      <c r="G9" s="272"/>
     </row>
     <row r="10" spans="1:11" ht="12.75" thickBot="1">
-      <c r="B10" s="218"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="220"/>
+      <c r="B10" s="274"/>
+      <c r="C10" s="275"/>
+      <c r="D10" s="275"/>
+      <c r="E10" s="275"/>
+      <c r="F10" s="275"/>
+      <c r="G10" s="276"/>
     </row>
     <row r="12" spans="1:11" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -11457,10 +11498,10 @@
       <c r="B24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="209" t="s">
+      <c r="C24" s="263" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="210"/>
+      <c r="D24" s="264"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -11478,10 +11519,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="249" t="s">
+      <c r="C25" s="302" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="250"/>
+      <c r="D25" s="303"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -11495,10 +11536,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="54"/>
-      <c r="C26" s="247" t="s">
+      <c r="C26" s="304" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="248"/>
+      <c r="D26" s="305"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58" t="s">
         <v>3</v>
@@ -11517,14 +11558,14 @@
       <c r="B29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="202" t="s">
+      <c r="C29" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="203"/>
-      <c r="E29" s="202" t="s">
+      <c r="D29" s="266"/>
+      <c r="E29" s="265" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="204"/>
+      <c r="F29" s="279"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -11541,14 +11582,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="202" t="s">
+      <c r="C32" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="203"/>
-      <c r="E32" s="202" t="s">
+      <c r="D32" s="266"/>
+      <c r="E32" s="265" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="204"/>
+      <c r="F32" s="279"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -11558,20 +11599,29 @@
         <v>1</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="245" t="s">
+      <c r="C33" s="306" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="246"/>
-      <c r="E33" s="247" t="s">
+      <c r="D33" s="307"/>
+      <c r="E33" s="304" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="248"/>
+      <c r="F33" s="305"/>
       <c r="G33" s="28" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -11584,15 +11634,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11640,105 +11681,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="256" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="228"/>
+      <c r="D2" s="257"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="223" t="s">
+      <c r="F2" s="256" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="224"/>
+      <c r="G2" s="260"/>
     </row>
     <row r="3" spans="1:7" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
+      <c r="C3" s="258"/>
+      <c r="D3" s="259"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="227" t="s">
+      <c r="F3" s="258" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="226"/>
+      <c r="G3" s="262"/>
     </row>
     <row r="4" spans="1:7" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="227" t="s">
+      <c r="C4" s="258" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="229"/>
+      <c r="D4" s="259"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="226"/>
+      <c r="F4" s="258"/>
+      <c r="G4" s="262"/>
     </row>
     <row r="5" spans="1:7" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="258" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="229"/>
+      <c r="D5" s="259"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="226"/>
+      <c r="F5" s="258"/>
+      <c r="G5" s="262"/>
     </row>
     <row r="6" spans="1:7" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="258" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="229"/>
+      <c r="D6" s="259"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="226"/>
+      <c r="F6" s="258"/>
+      <c r="G6" s="262"/>
     </row>
     <row r="7" spans="1:7" ht="14.25">
-      <c r="B7" s="211" t="s">
+      <c r="B7" s="267" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="212"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="213"/>
+      <c r="C7" s="268"/>
+      <c r="D7" s="268"/>
+      <c r="E7" s="268"/>
+      <c r="F7" s="268"/>
+      <c r="G7" s="269"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="214" t="s">
+      <c r="B8" s="270" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
+      <c r="C8" s="271"/>
+      <c r="D8" s="271"/>
+      <c r="E8" s="271"/>
+      <c r="F8" s="271"/>
+      <c r="G8" s="272"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="217"/>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="216"/>
+      <c r="B9" s="273"/>
+      <c r="C9" s="271"/>
+      <c r="D9" s="271"/>
+      <c r="E9" s="271"/>
+      <c r="F9" s="271"/>
+      <c r="G9" s="272"/>
     </row>
     <row r="10" spans="1:7" ht="12.75" thickBot="1">
-      <c r="B10" s="218"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="220"/>
+      <c r="B10" s="274"/>
+      <c r="C10" s="275"/>
+      <c r="D10" s="275"/>
+      <c r="E10" s="275"/>
+      <c r="F10" s="275"/>
+      <c r="G10" s="276"/>
     </row>
     <row r="12" spans="1:7" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -11843,10 +11884,10 @@
       <c r="B19" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="209" t="s">
+      <c r="C19" s="263" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="210"/>
+      <c r="D19" s="264"/>
       <c r="E19" s="34" t="s">
         <v>33</v>
       </c>
@@ -11864,10 +11905,10 @@
       <c r="B20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="249" t="s">
+      <c r="C20" s="302" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="250"/>
+      <c r="D20" s="303"/>
       <c r="E20" s="46" t="s">
         <v>3</v>
       </c>
@@ -11881,10 +11922,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="26"/>
-      <c r="C21" s="245" t="s">
+      <c r="C21" s="306" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="246"/>
+      <c r="D21" s="307"/>
       <c r="E21" s="45"/>
       <c r="F21" s="45" t="s">
         <v>3</v>
@@ -11903,14 +11944,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="202" t="s">
+      <c r="C24" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="203"/>
-      <c r="E24" s="202" t="s">
+      <c r="D24" s="266"/>
+      <c r="E24" s="265" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="204"/>
+      <c r="F24" s="279"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -11927,14 +11968,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="202" t="s">
+      <c r="C27" s="265" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="203"/>
-      <c r="E27" s="202" t="s">
+      <c r="D27" s="266"/>
+      <c r="E27" s="265" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="204"/>
+      <c r="F27" s="279"/>
       <c r="G27" s="38" t="s">
         <v>39</v>
       </c>
@@ -11944,14 +11985,23 @@
         <v>1</v>
       </c>
       <c r="B28" s="26"/>
-      <c r="C28" s="245"/>
-      <c r="D28" s="246"/>
-      <c r="E28" s="247"/>
-      <c r="F28" s="248"/>
+      <c r="C28" s="306"/>
+      <c r="D28" s="307"/>
+      <c r="E28" s="304"/>
+      <c r="F28" s="305"/>
       <c r="G28" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -11964,15 +12014,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
complete Api Specification design, change password size to 64
</commit_message>
<xml_diff>
--- a/doc/backend/db/TRN-MiniBlog_DatabaseDesign_LeDangHuy.xlsx
+++ b/doc/backend/db/TRN-MiniBlog_DatabaseDesign_LeDangHuy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14085" tabRatio="818" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14085" tabRatio="818" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="11" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="198">
   <si>
     <t>No</t>
   </si>
@@ -503,9 +503,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>VARCHAR(72)</t>
-  </si>
-  <si>
     <t>VARCHAR(32)</t>
   </si>
   <si>
@@ -690,6 +687,12 @@
   </si>
   <si>
     <t>fk_tokens_users1</t>
+  </si>
+  <si>
+    <t>VARCHAR(64)</t>
+  </si>
+  <si>
+    <t>token</t>
   </si>
 </sst>
 </file>
@@ -783,35 +786,49 @@
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <u/>
@@ -826,34 +843,46 @@
       <b/>
       <sz val="18"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3934,6 +3963,180 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4073,10 +4276,10 @@
     <xf numFmtId="49" fontId="29" fillId="2" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4085,10 +4288,19 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4108,189 +4320,6 @@
     </xf>
     <xf numFmtId="49" fontId="23" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="444">
@@ -6014,29 +6043,29 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="198"/>
-      <c r="P13" s="198"/>
-      <c r="Q13" s="198"/>
-      <c r="R13" s="198"/>
-      <c r="S13" s="198"/>
-      <c r="T13" s="198"/>
-      <c r="U13" s="198"/>
-      <c r="V13" s="198"/>
-      <c r="W13" s="198"/>
-      <c r="X13" s="198"/>
-      <c r="Y13" s="198"/>
-      <c r="Z13" s="198"/>
-      <c r="AA13" s="198"/>
-      <c r="AB13" s="198"/>
-      <c r="AC13" s="198"/>
-      <c r="AD13" s="198"/>
-      <c r="AE13" s="198"/>
-      <c r="AF13" s="198"/>
-      <c r="AG13" s="198"/>
-      <c r="AH13" s="198"/>
-      <c r="AI13" s="198"/>
-      <c r="AJ13" s="198"/>
-      <c r="AK13" s="198"/>
+      <c r="O13" s="256"/>
+      <c r="P13" s="256"/>
+      <c r="Q13" s="256"/>
+      <c r="R13" s="256"/>
+      <c r="S13" s="256"/>
+      <c r="T13" s="256"/>
+      <c r="U13" s="256"/>
+      <c r="V13" s="256"/>
+      <c r="W13" s="256"/>
+      <c r="X13" s="256"/>
+      <c r="Y13" s="256"/>
+      <c r="Z13" s="256"/>
+      <c r="AA13" s="256"/>
+      <c r="AB13" s="256"/>
+      <c r="AC13" s="256"/>
+      <c r="AD13" s="256"/>
+      <c r="AE13" s="256"/>
+      <c r="AF13" s="256"/>
+      <c r="AG13" s="256"/>
+      <c r="AH13" s="256"/>
+      <c r="AI13" s="256"/>
+      <c r="AJ13" s="256"/>
+      <c r="AK13" s="256"/>
       <c r="AL13" s="4"/>
       <c r="AM13" s="4"/>
       <c r="AN13" s="4"/>
@@ -6068,29 +6097,29 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="198"/>
-      <c r="P14" s="198"/>
-      <c r="Q14" s="198"/>
-      <c r="R14" s="198"/>
-      <c r="S14" s="198"/>
-      <c r="T14" s="198"/>
-      <c r="U14" s="198"/>
-      <c r="V14" s="198"/>
-      <c r="W14" s="198"/>
-      <c r="X14" s="198"/>
-      <c r="Y14" s="198"/>
-      <c r="Z14" s="198"/>
-      <c r="AA14" s="198"/>
-      <c r="AB14" s="198"/>
-      <c r="AC14" s="198"/>
-      <c r="AD14" s="198"/>
-      <c r="AE14" s="198"/>
-      <c r="AF14" s="198"/>
-      <c r="AG14" s="198"/>
-      <c r="AH14" s="198"/>
-      <c r="AI14" s="198"/>
-      <c r="AJ14" s="198"/>
-      <c r="AK14" s="198"/>
+      <c r="O14" s="256"/>
+      <c r="P14" s="256"/>
+      <c r="Q14" s="256"/>
+      <c r="R14" s="256"/>
+      <c r="S14" s="256"/>
+      <c r="T14" s="256"/>
+      <c r="U14" s="256"/>
+      <c r="V14" s="256"/>
+      <c r="W14" s="256"/>
+      <c r="X14" s="256"/>
+      <c r="Y14" s="256"/>
+      <c r="Z14" s="256"/>
+      <c r="AA14" s="256"/>
+      <c r="AB14" s="256"/>
+      <c r="AC14" s="256"/>
+      <c r="AD14" s="256"/>
+      <c r="AE14" s="256"/>
+      <c r="AF14" s="256"/>
+      <c r="AG14" s="256"/>
+      <c r="AH14" s="256"/>
+      <c r="AI14" s="256"/>
+      <c r="AJ14" s="256"/>
+      <c r="AK14" s="256"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
@@ -6118,43 +6147,43 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="199" t="s">
+      <c r="K15" s="257" t="s">
         <v>119</v>
       </c>
-      <c r="L15" s="199"/>
-      <c r="M15" s="199"/>
-      <c r="N15" s="199"/>
-      <c r="O15" s="199"/>
-      <c r="P15" s="199"/>
-      <c r="Q15" s="199"/>
-      <c r="R15" s="199"/>
-      <c r="S15" s="199"/>
-      <c r="T15" s="199"/>
-      <c r="U15" s="199"/>
-      <c r="V15" s="199"/>
-      <c r="W15" s="199"/>
-      <c r="X15" s="199"/>
-      <c r="Y15" s="199"/>
-      <c r="Z15" s="199"/>
-      <c r="AA15" s="199"/>
-      <c r="AB15" s="199"/>
-      <c r="AC15" s="199"/>
-      <c r="AD15" s="199"/>
-      <c r="AE15" s="199"/>
-      <c r="AF15" s="199"/>
-      <c r="AG15" s="199"/>
-      <c r="AH15" s="199"/>
-      <c r="AI15" s="199"/>
-      <c r="AJ15" s="199"/>
-      <c r="AK15" s="199"/>
-      <c r="AL15" s="199"/>
-      <c r="AM15" s="199"/>
-      <c r="AN15" s="199"/>
-      <c r="AO15" s="199"/>
-      <c r="AP15" s="199"/>
-      <c r="AQ15" s="199"/>
-      <c r="AR15" s="199"/>
-      <c r="AS15" s="199"/>
+      <c r="L15" s="257"/>
+      <c r="M15" s="257"/>
+      <c r="N15" s="257"/>
+      <c r="O15" s="257"/>
+      <c r="P15" s="257"/>
+      <c r="Q15" s="257"/>
+      <c r="R15" s="257"/>
+      <c r="S15" s="257"/>
+      <c r="T15" s="257"/>
+      <c r="U15" s="257"/>
+      <c r="V15" s="257"/>
+      <c r="W15" s="257"/>
+      <c r="X15" s="257"/>
+      <c r="Y15" s="257"/>
+      <c r="Z15" s="257"/>
+      <c r="AA15" s="257"/>
+      <c r="AB15" s="257"/>
+      <c r="AC15" s="257"/>
+      <c r="AD15" s="257"/>
+      <c r="AE15" s="257"/>
+      <c r="AF15" s="257"/>
+      <c r="AG15" s="257"/>
+      <c r="AH15" s="257"/>
+      <c r="AI15" s="257"/>
+      <c r="AJ15" s="257"/>
+      <c r="AK15" s="257"/>
+      <c r="AL15" s="257"/>
+      <c r="AM15" s="257"/>
+      <c r="AN15" s="257"/>
+      <c r="AO15" s="257"/>
+      <c r="AP15" s="257"/>
+      <c r="AQ15" s="257"/>
+      <c r="AR15" s="257"/>
+      <c r="AS15" s="257"/>
       <c r="AT15" s="4"/>
       <c r="AU15" s="4"/>
       <c r="AV15" s="4"/>
@@ -6174,41 +6203,41 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="199"/>
-      <c r="L16" s="199"/>
-      <c r="M16" s="199"/>
-      <c r="N16" s="199"/>
-      <c r="O16" s="199"/>
-      <c r="P16" s="199"/>
-      <c r="Q16" s="199"/>
-      <c r="R16" s="199"/>
-      <c r="S16" s="199"/>
-      <c r="T16" s="199"/>
-      <c r="U16" s="199"/>
-      <c r="V16" s="199"/>
-      <c r="W16" s="199"/>
-      <c r="X16" s="199"/>
-      <c r="Y16" s="199"/>
-      <c r="Z16" s="199"/>
-      <c r="AA16" s="199"/>
-      <c r="AB16" s="199"/>
-      <c r="AC16" s="199"/>
-      <c r="AD16" s="199"/>
-      <c r="AE16" s="199"/>
-      <c r="AF16" s="199"/>
-      <c r="AG16" s="199"/>
-      <c r="AH16" s="199"/>
-      <c r="AI16" s="199"/>
-      <c r="AJ16" s="199"/>
-      <c r="AK16" s="199"/>
-      <c r="AL16" s="199"/>
-      <c r="AM16" s="199"/>
-      <c r="AN16" s="199"/>
-      <c r="AO16" s="199"/>
-      <c r="AP16" s="199"/>
-      <c r="AQ16" s="199"/>
-      <c r="AR16" s="199"/>
-      <c r="AS16" s="199"/>
+      <c r="K16" s="257"/>
+      <c r="L16" s="257"/>
+      <c r="M16" s="257"/>
+      <c r="N16" s="257"/>
+      <c r="O16" s="257"/>
+      <c r="P16" s="257"/>
+      <c r="Q16" s="257"/>
+      <c r="R16" s="257"/>
+      <c r="S16" s="257"/>
+      <c r="T16" s="257"/>
+      <c r="U16" s="257"/>
+      <c r="V16" s="257"/>
+      <c r="W16" s="257"/>
+      <c r="X16" s="257"/>
+      <c r="Y16" s="257"/>
+      <c r="Z16" s="257"/>
+      <c r="AA16" s="257"/>
+      <c r="AB16" s="257"/>
+      <c r="AC16" s="257"/>
+      <c r="AD16" s="257"/>
+      <c r="AE16" s="257"/>
+      <c r="AF16" s="257"/>
+      <c r="AG16" s="257"/>
+      <c r="AH16" s="257"/>
+      <c r="AI16" s="257"/>
+      <c r="AJ16" s="257"/>
+      <c r="AK16" s="257"/>
+      <c r="AL16" s="257"/>
+      <c r="AM16" s="257"/>
+      <c r="AN16" s="257"/>
+      <c r="AO16" s="257"/>
+      <c r="AP16" s="257"/>
+      <c r="AQ16" s="257"/>
+      <c r="AR16" s="257"/>
+      <c r="AS16" s="257"/>
       <c r="AT16" s="4"/>
       <c r="AU16" s="4"/>
       <c r="AV16" s="4"/>
@@ -6797,14 +6826,14 @@
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
       <c r="AM27" s="7"/>
-      <c r="AN27" s="200">
+      <c r="AN27" s="258">
         <v>41922</v>
       </c>
-      <c r="AO27" s="200"/>
-      <c r="AP27" s="200"/>
-      <c r="AQ27" s="200"/>
-      <c r="AR27" s="200"/>
-      <c r="AS27" s="200"/>
+      <c r="AO27" s="258"/>
+      <c r="AP27" s="258"/>
+      <c r="AQ27" s="258"/>
+      <c r="AR27" s="258"/>
+      <c r="AS27" s="258"/>
       <c r="AT27" s="12"/>
       <c r="AU27" s="12"/>
       <c r="AV27" s="12"/>
@@ -7294,103 +7323,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="281" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="228"/>
+      <c r="D2" s="286"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="255" t="s">
+      <c r="F2" s="316" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="256"/>
+      <c r="G2" s="317"/>
     </row>
     <row r="3" spans="1:14" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
+      <c r="C3" s="285"/>
+      <c r="D3" s="287"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="225" t="s">
+      <c r="F3" s="283" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="226"/>
+      <c r="G3" s="284"/>
     </row>
     <row r="4" spans="1:14" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="227" t="s">
+      <c r="C4" s="285" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="229"/>
+      <c r="D4" s="287"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="226"/>
+      <c r="F4" s="285"/>
+      <c r="G4" s="284"/>
     </row>
     <row r="5" spans="1:14" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="285" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="229"/>
+      <c r="D5" s="287"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="226"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="284"/>
     </row>
     <row r="6" spans="1:14" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="285" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="229"/>
+      <c r="D6" s="287"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="226"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="284"/>
     </row>
     <row r="7" spans="1:14" ht="14.25">
-      <c r="B7" s="211" t="s">
+      <c r="B7" s="269" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="212"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="213"/>
+      <c r="C7" s="270"/>
+      <c r="D7" s="270"/>
+      <c r="E7" s="270"/>
+      <c r="F7" s="270"/>
+      <c r="G7" s="271"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="214"/>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
+      <c r="B8" s="272"/>
+      <c r="C8" s="273"/>
+      <c r="D8" s="273"/>
+      <c r="E8" s="273"/>
+      <c r="F8" s="273"/>
+      <c r="G8" s="274"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="217"/>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="216"/>
+      <c r="B9" s="275"/>
+      <c r="C9" s="273"/>
+      <c r="D9" s="273"/>
+      <c r="E9" s="273"/>
+      <c r="F9" s="273"/>
+      <c r="G9" s="274"/>
     </row>
     <row r="10" spans="1:14" ht="12.75" thickBot="1">
-      <c r="B10" s="218"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="220"/>
+      <c r="B10" s="276"/>
+      <c r="C10" s="277"/>
+      <c r="D10" s="277"/>
+      <c r="E10" s="277"/>
+      <c r="F10" s="277"/>
+      <c r="G10" s="278"/>
     </row>
     <row r="11" spans="1:14">
       <c r="H11" s="87"/>
@@ -7606,10 +7635,10 @@
       <c r="B21" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="209" t="s">
+      <c r="C21" s="267" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="210"/>
+      <c r="D21" s="268"/>
       <c r="E21" s="34" t="s">
         <v>33</v>
       </c>
@@ -7633,10 +7662,10 @@
       <c r="B22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="249" t="s">
+      <c r="C22" s="303" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="250"/>
+      <c r="D22" s="304"/>
       <c r="E22" s="46" t="s">
         <v>3</v>
       </c>
@@ -7656,10 +7685,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="253" t="s">
+      <c r="C23" s="314" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="254"/>
+      <c r="D23" s="315"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
         <v>3</v>
@@ -7677,10 +7706,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="26"/>
-      <c r="C24" s="245" t="s">
+      <c r="C24" s="310" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="246"/>
+      <c r="D24" s="311"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45" t="s">
         <v>3</v>
@@ -7719,14 +7748,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="202" t="s">
+      <c r="C27" s="260" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="203"/>
-      <c r="E27" s="202" t="s">
+      <c r="D27" s="261"/>
+      <c r="E27" s="260" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="204"/>
+      <c r="F27" s="262"/>
       <c r="G27" s="38" t="s">
         <v>38</v>
       </c>
@@ -7763,14 +7792,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="202" t="s">
+      <c r="C30" s="260" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="203"/>
-      <c r="E30" s="202" t="s">
+      <c r="D30" s="261"/>
+      <c r="E30" s="260" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="204"/>
+      <c r="F30" s="262"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
@@ -7786,14 +7815,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="249" t="s">
+      <c r="C31" s="303" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="250"/>
-      <c r="E31" s="253" t="s">
+      <c r="D31" s="304"/>
+      <c r="E31" s="314" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="254"/>
+      <c r="F31" s="315"/>
       <c r="G31" s="53" t="s">
         <v>76</v>
       </c>
@@ -7809,14 +7838,14 @@
         <v>2</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="251" t="s">
+      <c r="C32" s="312" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="252"/>
-      <c r="E32" s="247" t="s">
+      <c r="D32" s="313"/>
+      <c r="E32" s="305" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="248"/>
+      <c r="F32" s="306"/>
       <c r="G32" s="55" t="s">
         <v>52</v>
       </c>
@@ -7914,7 +7943,7 @@
   <dimension ref="B1:F34"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -7950,7 +7979,7 @@
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="93">
-        <v>41922</v>
+        <v>42031</v>
       </c>
       <c r="C3" s="114" t="s">
         <v>103</v>
@@ -8198,7 +8227,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
@@ -8209,11 +8238,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" thickBot="1">
-      <c r="A1" s="201" t="s">
+      <c r="A1" s="259" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
+      <c r="B1" s="259"/>
+      <c r="C1" s="259"/>
     </row>
     <row r="2" spans="1:3" ht="12.75" thickBot="1">
       <c r="A2" s="118" t="s">
@@ -8249,7 +8278,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1">
       <c r="A5" s="59">
         <f t="shared" ref="A5:A28" si="0">A4+1</f>
         <v>3</v>
@@ -8261,13 +8290,17 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" ht="15">
       <c r="A6" s="59">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="123"/>
-      <c r="C6" s="124"/>
+      <c r="B6" s="123" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" s="135" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="59">
@@ -8454,6 +8487,7 @@
     <hyperlink ref="C3" location="user!A1" display="user"/>
     <hyperlink ref="C4" location="posts!A1" display="posts"/>
     <hyperlink ref="C5" location="comments!A1" display="comments"/>
+    <hyperlink ref="C6" location="token!A1" display="token"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
@@ -8476,8 +8510,8 @@
   </sheetPr>
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
@@ -8508,103 +8542,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="281" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="228"/>
+      <c r="D2" s="286"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="223" t="s">
+      <c r="F2" s="281" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="224"/>
+      <c r="G2" s="282"/>
     </row>
     <row r="3" spans="1:19" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
+      <c r="C3" s="285"/>
+      <c r="D3" s="287"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="225" t="s">
-        <v>150</v>
-      </c>
-      <c r="G3" s="226"/>
+      <c r="F3" s="283" t="s">
+        <v>149</v>
+      </c>
+      <c r="G3" s="284"/>
     </row>
     <row r="4" spans="1:19" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="227" t="s">
+      <c r="C4" s="285" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="229"/>
+      <c r="D4" s="287"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="226"/>
+      <c r="F4" s="285"/>
+      <c r="G4" s="284"/>
     </row>
     <row r="5" spans="1:19" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="285" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="229"/>
+      <c r="D5" s="287"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="226"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="284"/>
     </row>
     <row r="6" spans="1:19" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="285" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="229"/>
+      <c r="D6" s="287"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="226"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="284"/>
     </row>
     <row r="7" spans="1:19" ht="14.25">
-      <c r="B7" s="211" t="s">
+      <c r="B7" s="269" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="212"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="213"/>
+      <c r="C7" s="270"/>
+      <c r="D7" s="270"/>
+      <c r="E7" s="270"/>
+      <c r="F7" s="270"/>
+      <c r="G7" s="271"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="214"/>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
+      <c r="B8" s="272"/>
+      <c r="C8" s="273"/>
+      <c r="D8" s="273"/>
+      <c r="E8" s="273"/>
+      <c r="F8" s="273"/>
+      <c r="G8" s="274"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="217"/>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="216"/>
+      <c r="B9" s="275"/>
+      <c r="C9" s="273"/>
+      <c r="D9" s="273"/>
+      <c r="E9" s="273"/>
+      <c r="F9" s="273"/>
+      <c r="G9" s="274"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" thickBot="1">
-      <c r="B10" s="218"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="220"/>
+      <c r="B10" s="276"/>
+      <c r="C10" s="277"/>
+      <c r="D10" s="277"/>
+      <c r="E10" s="277"/>
+      <c r="F10" s="277"/>
+      <c r="G10" s="278"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8679,7 +8713,7 @@
         <v>114</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E14" s="66" t="s">
         <v>3</v>
@@ -8732,7 +8766,7 @@
         <v>107</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -8785,14 +8819,14 @@
         <v>116</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="136" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H16" s="87"/>
     </row>
@@ -8802,20 +8836,20 @@
         <v>4</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="117" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -8824,20 +8858,20 @@
         <v>5</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D18" s="129" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="106" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -8846,20 +8880,20 @@
         <v>6</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F19" s="67"/>
       <c r="G19" s="106" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -8868,19 +8902,19 @@
         <v>7</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C20" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D20" s="65" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E20" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="162" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G20" s="106" t="s">
         <v>100</v>
@@ -8892,22 +8926,22 @@
         <v>8</v>
       </c>
       <c r="B21" s="131" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C21" s="132" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D21" s="68" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E21" s="133" t="s">
         <v>3</v>
       </c>
       <c r="F21" s="163" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G21" s="137" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="12.75" thickBot="1">
@@ -8922,10 +8956,10 @@
       <c r="B25" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="209" t="s">
+      <c r="C25" s="267" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="210"/>
+      <c r="D25" s="268"/>
       <c r="E25" s="34" t="s">
         <v>33</v>
       </c>
@@ -8943,10 +8977,10 @@
       <c r="B26" s="166" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="221" t="s">
+      <c r="C26" s="279" t="s">
         <v>114</v>
       </c>
-      <c r="D26" s="222"/>
+      <c r="D26" s="280"/>
       <c r="E26" s="167" t="s">
         <v>3</v>
       </c>
@@ -8962,16 +8996,16 @@
       <c r="B27" s="155" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="207" t="s">
+      <c r="C27" s="265" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="208"/>
+      <c r="D27" s="266"/>
       <c r="E27" s="169"/>
       <c r="F27" s="44" t="s">
         <v>3</v>
       </c>
       <c r="G27" s="161" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="12.95" customHeight="1">
@@ -8979,10 +9013,10 @@
         <v>3</v>
       </c>
       <c r="B28" s="155" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C28" s="170" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D28" s="171"/>
       <c r="E28" s="44"/>
@@ -8994,8 +9028,8 @@
     <row r="29" spans="1:7" ht="12.95" customHeight="1" thickBot="1">
       <c r="A29" s="16"/>
       <c r="B29" s="172"/>
-      <c r="C29" s="205"/>
-      <c r="D29" s="206"/>
+      <c r="C29" s="263"/>
+      <c r="D29" s="264"/>
       <c r="E29" s="45"/>
       <c r="F29" s="45"/>
       <c r="G29" s="28"/>
@@ -9012,14 +9046,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="202" t="s">
+      <c r="C32" s="260" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="203"/>
-      <c r="E32" s="202" t="s">
+      <c r="D32" s="261"/>
+      <c r="E32" s="260" t="s">
         <v>36</v>
       </c>
-      <c r="F32" s="204"/>
+      <c r="F32" s="262"/>
       <c r="G32" s="38" t="s">
         <v>38</v>
       </c>
@@ -9036,14 +9070,14 @@
       <c r="B35" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="202" t="s">
+      <c r="C35" s="260" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="203"/>
-      <c r="E35" s="202" t="s">
+      <c r="D35" s="261"/>
+      <c r="E35" s="260" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="204"/>
+      <c r="F35" s="262"/>
       <c r="G35" s="38" t="s">
         <v>39</v>
       </c>
@@ -9122,103 +9156,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="281" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="228"/>
+      <c r="D2" s="286"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="223" t="s">
+      <c r="F2" s="281" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="224"/>
+      <c r="G2" s="282"/>
     </row>
     <row r="3" spans="1:19" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
+      <c r="C3" s="285"/>
+      <c r="D3" s="287"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="225" t="s">
-        <v>150</v>
-      </c>
-      <c r="G3" s="226"/>
+      <c r="F3" s="283" t="s">
+        <v>149</v>
+      </c>
+      <c r="G3" s="284"/>
     </row>
     <row r="4" spans="1:19" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="227" t="s">
+      <c r="C4" s="285" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="229"/>
+      <c r="D4" s="287"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="226"/>
+      <c r="F4" s="285"/>
+      <c r="G4" s="284"/>
     </row>
     <row r="5" spans="1:19" ht="14.25">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="285" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="229"/>
+      <c r="D5" s="287"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="226"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="284"/>
     </row>
     <row r="6" spans="1:19" ht="14.25">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="285" t="s">
         <v>129</v>
       </c>
-      <c r="D6" s="229"/>
+      <c r="D6" s="287"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="226"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="284"/>
     </row>
     <row r="7" spans="1:19" ht="14.25">
-      <c r="B7" s="211" t="s">
+      <c r="B7" s="269" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="212"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="213"/>
+      <c r="C7" s="270"/>
+      <c r="D7" s="270"/>
+      <c r="E7" s="270"/>
+      <c r="F7" s="270"/>
+      <c r="G7" s="271"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="214"/>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
+      <c r="B8" s="272"/>
+      <c r="C8" s="273"/>
+      <c r="D8" s="273"/>
+      <c r="E8" s="273"/>
+      <c r="F8" s="273"/>
+      <c r="G8" s="274"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="217"/>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="216"/>
+      <c r="B9" s="275"/>
+      <c r="C9" s="273"/>
+      <c r="D9" s="273"/>
+      <c r="E9" s="273"/>
+      <c r="F9" s="273"/>
+      <c r="G9" s="274"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" thickBot="1">
-      <c r="B10" s="218"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="220"/>
+      <c r="B10" s="276"/>
+      <c r="C10" s="277"/>
+      <c r="D10" s="277"/>
+      <c r="E10" s="277"/>
+      <c r="F10" s="277"/>
+      <c r="G10" s="278"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9293,7 +9327,7 @@
         <v>114</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E14" s="66" t="s">
         <v>3</v>
@@ -9340,13 +9374,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
+        <v>152</v>
+      </c>
+      <c r="C15" s="65" t="s">
         <v>153</v>
       </c>
-      <c r="C15" s="65" t="s">
+      <c r="D15" s="65" t="s">
         <v>154</v>
-      </c>
-      <c r="D15" s="65" t="s">
-        <v>155</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -9394,10 +9428,10 @@
         <v>12</v>
       </c>
       <c r="C16" s="65" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="65" t="s">
         <v>156</v>
-      </c>
-      <c r="D16" s="65" t="s">
-        <v>157</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
@@ -9412,19 +9446,19 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="162" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G17" s="106" t="s">
         <v>100</v>
@@ -9436,22 +9470,22 @@
         <v>5</v>
       </c>
       <c r="B18" s="150" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C18" s="151" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D18" s="152" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E18" s="153" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="164" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G18" s="154" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -9473,7 +9507,7 @@
       </c>
       <c r="F19" s="22"/>
       <c r="G19" s="161" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="12.75" thickBot="1">
@@ -9482,20 +9516,20 @@
         <v>7</v>
       </c>
       <c r="B20" s="157" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" s="158" t="s">
         <v>158</v>
       </c>
-      <c r="C20" s="158" t="s">
-        <v>159</v>
-      </c>
       <c r="D20" s="159" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E20" s="133" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="160"/>
       <c r="G20" s="137" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -9546,10 +9580,10 @@
       <c r="B27" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="209" t="s">
+      <c r="C27" s="267" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="210"/>
+      <c r="D27" s="268"/>
       <c r="E27" s="34" t="s">
         <v>33</v>
       </c>
@@ -9567,10 +9601,10 @@
       <c r="B28" s="186" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="230" t="s">
+      <c r="C28" s="288" t="s">
         <v>114</v>
       </c>
-      <c r="D28" s="231"/>
+      <c r="D28" s="289"/>
       <c r="E28" s="187" t="s">
         <v>3</v>
       </c>
@@ -9584,12 +9618,12 @@
         <v>2</v>
       </c>
       <c r="B29" s="191" t="s">
-        <v>154</v>
-      </c>
-      <c r="C29" s="232" t="s">
-        <v>154</v>
-      </c>
-      <c r="D29" s="233"/>
+        <v>153</v>
+      </c>
+      <c r="C29" s="290" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" s="291"/>
       <c r="E29" s="192"/>
       <c r="F29" s="192"/>
       <c r="G29" s="193"/>
@@ -9599,12 +9633,12 @@
         <v>3</v>
       </c>
       <c r="B30" s="195" t="s">
-        <v>165</v>
-      </c>
-      <c r="C30" s="234" t="s">
-        <v>159</v>
-      </c>
-      <c r="D30" s="235"/>
+        <v>164</v>
+      </c>
+      <c r="C30" s="292" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" s="293"/>
       <c r="E30" s="196" t="s">
         <v>3</v>
       </c>
@@ -9628,14 +9662,14 @@
       <c r="B34" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="202" t="s">
+      <c r="C34" s="260" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="203"/>
-      <c r="E34" s="202" t="s">
+      <c r="D34" s="261"/>
+      <c r="E34" s="260" t="s">
         <v>36</v>
       </c>
-      <c r="F34" s="204"/>
+      <c r="F34" s="262"/>
       <c r="G34" s="38" t="s">
         <v>38</v>
       </c>
@@ -9645,14 +9679,14 @@
         <v>1</v>
       </c>
       <c r="B35" s="174" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C35" s="174"/>
       <c r="D35" s="174"/>
-      <c r="E35" s="236" t="s">
-        <v>167</v>
-      </c>
-      <c r="F35" s="237"/>
+      <c r="E35" s="294" t="s">
+        <v>166</v>
+      </c>
+      <c r="F35" s="295"/>
       <c r="G35" s="175"/>
     </row>
     <row r="37" spans="1:7" ht="12.75" thickBot="1">
@@ -9667,14 +9701,14 @@
       <c r="B38" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="202" t="s">
+      <c r="C38" s="260" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="203"/>
-      <c r="E38" s="202" t="s">
+      <c r="D38" s="261"/>
+      <c r="E38" s="260" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="204"/>
+      <c r="F38" s="262"/>
       <c r="G38" s="38" t="s">
         <v>39</v>
       </c>
@@ -9744,103 +9778,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="281" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="228"/>
+      <c r="D2" s="286"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="223" t="s">
+      <c r="F2" s="281" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="224"/>
+      <c r="G2" s="282"/>
     </row>
     <row r="3" spans="1:19" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
+      <c r="C3" s="285"/>
+      <c r="D3" s="287"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="238" t="s">
-        <v>150</v>
-      </c>
-      <c r="G3" s="226"/>
+      <c r="F3" s="296" t="s">
+        <v>149</v>
+      </c>
+      <c r="G3" s="284"/>
     </row>
     <row r="4" spans="1:19" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="227" t="s">
+      <c r="C4" s="285" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="229"/>
+      <c r="D4" s="287"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="226"/>
+      <c r="F4" s="285"/>
+      <c r="G4" s="284"/>
     </row>
     <row r="5" spans="1:19" ht="14.25">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="285" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="229"/>
+      <c r="D5" s="287"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="226"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="284"/>
     </row>
     <row r="6" spans="1:19" ht="14.25">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="285" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="229"/>
+      <c r="D6" s="287"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="226"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="284"/>
     </row>
     <row r="7" spans="1:19" ht="14.25">
-      <c r="B7" s="211" t="s">
+      <c r="B7" s="269" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="212"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="213"/>
+      <c r="C7" s="270"/>
+      <c r="D7" s="270"/>
+      <c r="E7" s="270"/>
+      <c r="F7" s="270"/>
+      <c r="G7" s="271"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="214"/>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
+      <c r="B8" s="272"/>
+      <c r="C8" s="273"/>
+      <c r="D8" s="273"/>
+      <c r="E8" s="273"/>
+      <c r="F8" s="273"/>
+      <c r="G8" s="274"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="217"/>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="216"/>
+      <c r="B9" s="275"/>
+      <c r="C9" s="273"/>
+      <c r="D9" s="273"/>
+      <c r="E9" s="273"/>
+      <c r="F9" s="273"/>
+      <c r="G9" s="274"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" thickBot="1">
-      <c r="B10" s="218"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="220"/>
+      <c r="B10" s="276"/>
+      <c r="C10" s="277"/>
+      <c r="D10" s="277"/>
+      <c r="E10" s="277"/>
+      <c r="F10" s="277"/>
+      <c r="G10" s="278"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9915,7 +9949,7 @@
         <v>114</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E14" s="66" t="s">
         <v>3</v>
@@ -9962,13 +9996,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="176" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" s="177" t="s">
         <v>168</v>
       </c>
-      <c r="C15" s="177" t="s">
-        <v>169</v>
-      </c>
       <c r="D15" s="177" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -10015,13 +10049,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="176" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="177" t="s">
         <v>170</v>
       </c>
-      <c r="C16" s="177" t="s">
-        <v>171</v>
-      </c>
       <c r="D16" s="177" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
@@ -10036,13 +10070,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="176" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="177" t="s">
         <v>158</v>
       </c>
-      <c r="C17" s="177" t="s">
-        <v>159</v>
-      </c>
       <c r="D17" s="177" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
@@ -10056,19 +10090,19 @@
         <v>5</v>
       </c>
       <c r="B18" s="176" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C18" s="177" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="162" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G18" s="106" t="s">
         <v>100</v>
@@ -10080,22 +10114,22 @@
         <v>6</v>
       </c>
       <c r="B19" s="157" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C19" s="158" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D19" s="68" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E19" s="133" t="s">
         <v>3</v>
       </c>
       <c r="F19" s="178" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G19" s="137" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75" thickBot="1">
@@ -10110,10 +10144,10 @@
       <c r="B22" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="209" t="s">
+      <c r="C22" s="267" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="210"/>
+      <c r="D22" s="268"/>
       <c r="E22" s="34" t="s">
         <v>33</v>
       </c>
@@ -10131,10 +10165,10 @@
       <c r="B23" s="166" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="221" t="s">
+      <c r="C23" s="279" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="222"/>
+      <c r="D23" s="280"/>
       <c r="E23" s="167" t="s">
         <v>3</v>
       </c>
@@ -10148,12 +10182,12 @@
         <v>2</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="C24" s="207" t="s">
-        <v>171</v>
-      </c>
-      <c r="D24" s="208"/>
+        <v>173</v>
+      </c>
+      <c r="C24" s="265" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24" s="266"/>
       <c r="E24" s="44"/>
       <c r="F24" s="44"/>
       <c r="G24" s="24"/>
@@ -10163,12 +10197,12 @@
         <v>3</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>175</v>
-      </c>
-      <c r="C25" s="205" t="s">
-        <v>159</v>
-      </c>
-      <c r="D25" s="206"/>
+        <v>174</v>
+      </c>
+      <c r="C25" s="263" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="264"/>
       <c r="E25" s="45"/>
       <c r="F25" s="45"/>
       <c r="G25" s="28"/>
@@ -10185,14 +10219,14 @@
       <c r="B28" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="202" t="s">
+      <c r="C28" s="260" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="203"/>
-      <c r="E28" s="202" t="s">
+      <c r="D28" s="261"/>
+      <c r="E28" s="260" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="204"/>
+      <c r="F28" s="262"/>
       <c r="G28" s="38" t="s">
         <v>38</v>
       </c>
@@ -10202,14 +10236,14 @@
         <v>1</v>
       </c>
       <c r="B29" s="180" t="s">
-        <v>176</v>
-      </c>
-      <c r="C29" s="243"/>
-      <c r="D29" s="244"/>
-      <c r="E29" s="239" t="s">
-        <v>178</v>
-      </c>
-      <c r="F29" s="239"/>
+        <v>175</v>
+      </c>
+      <c r="C29" s="301"/>
+      <c r="D29" s="302"/>
+      <c r="E29" s="297" t="s">
+        <v>177</v>
+      </c>
+      <c r="F29" s="297"/>
       <c r="G29" s="181"/>
     </row>
     <row r="30" spans="1:7" ht="14.25" customHeight="1" thickBot="1">
@@ -10217,14 +10251,14 @@
         <v>2</v>
       </c>
       <c r="B30" s="183" t="s">
-        <v>177</v>
-      </c>
-      <c r="C30" s="241"/>
-      <c r="D30" s="242"/>
-      <c r="E30" s="240" t="s">
-        <v>167</v>
-      </c>
-      <c r="F30" s="240"/>
+        <v>176</v>
+      </c>
+      <c r="C30" s="299"/>
+      <c r="D30" s="300"/>
+      <c r="E30" s="298" t="s">
+        <v>166</v>
+      </c>
+      <c r="F30" s="298"/>
       <c r="G30" s="184"/>
     </row>
     <row r="32" spans="1:7" ht="12.75" thickBot="1">
@@ -10239,14 +10273,14 @@
       <c r="B33" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="202" t="s">
+      <c r="C33" s="260" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="203"/>
-      <c r="E33" s="202" t="s">
+      <c r="D33" s="261"/>
+      <c r="E33" s="260" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="204"/>
+      <c r="F33" s="262"/>
       <c r="G33" s="38" t="s">
         <v>39</v>
       </c>
@@ -10286,8 +10320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10303,779 +10337,779 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="200" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="261"/>
-      <c r="C1" s="261"/>
-      <c r="D1" s="261"/>
-      <c r="E1" s="261"/>
-      <c r="F1" s="261"/>
-      <c r="G1" s="261"/>
-      <c r="H1" s="261"/>
-      <c r="I1" s="261"/>
-      <c r="J1" s="261"/>
-      <c r="K1" s="261"/>
-      <c r="L1" s="261"/>
-      <c r="M1" s="261"/>
-      <c r="N1" s="261"/>
-      <c r="O1" s="261"/>
-      <c r="P1" s="261"/>
-      <c r="Q1" s="261"/>
-      <c r="R1" s="261"/>
-      <c r="S1" s="261"/>
-      <c r="T1" s="261"/>
-      <c r="U1" s="261"/>
-      <c r="V1" s="261"/>
-    </row>
-    <row r="2" spans="1:22" ht="24">
-      <c r="A2" s="261"/>
-      <c r="B2" s="277" t="s">
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="199"/>
+      <c r="I1" s="199"/>
+      <c r="J1" s="199"/>
+      <c r="K1" s="199"/>
+      <c r="L1" s="199"/>
+      <c r="M1" s="199"/>
+      <c r="N1" s="199"/>
+      <c r="O1" s="199"/>
+      <c r="P1" s="199"/>
+      <c r="Q1" s="199"/>
+      <c r="R1" s="199"/>
+      <c r="S1" s="199"/>
+      <c r="T1" s="199"/>
+      <c r="U1" s="199"/>
+      <c r="V1" s="199"/>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="199"/>
+      <c r="B2" s="215" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="223" t="s">
-        <v>193</v>
-      </c>
-      <c r="D2" s="228"/>
-      <c r="E2" s="279" t="s">
+      <c r="C2" s="281" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="286"/>
+      <c r="E2" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="223" t="s">
+      <c r="F2" s="281" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="224"/>
-      <c r="H2" s="261"/>
-      <c r="I2" s="261"/>
-      <c r="J2" s="261"/>
-      <c r="K2" s="261"/>
-      <c r="L2" s="261"/>
-      <c r="M2" s="261"/>
-      <c r="N2" s="261"/>
-      <c r="O2" s="261"/>
-      <c r="P2" s="261"/>
-      <c r="Q2" s="261"/>
-      <c r="R2" s="261"/>
-      <c r="S2" s="261"/>
-      <c r="T2" s="261"/>
-      <c r="U2" s="261"/>
-      <c r="V2" s="261"/>
-    </row>
-    <row r="3" spans="1:22" ht="36">
-      <c r="A3" s="261"/>
-      <c r="B3" s="278" t="s">
+      <c r="G2" s="282"/>
+      <c r="H2" s="199"/>
+      <c r="I2" s="199"/>
+      <c r="J2" s="199"/>
+      <c r="K2" s="199"/>
+      <c r="L2" s="199"/>
+      <c r="M2" s="199"/>
+      <c r="N2" s="199"/>
+      <c r="O2" s="199"/>
+      <c r="P2" s="199"/>
+      <c r="Q2" s="199"/>
+      <c r="R2" s="199"/>
+      <c r="S2" s="199"/>
+      <c r="T2" s="199"/>
+      <c r="U2" s="199"/>
+      <c r="V2" s="199"/>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="199"/>
+      <c r="B3" s="216" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
-      <c r="E3" s="280" t="s">
+      <c r="C3" s="285"/>
+      <c r="D3" s="287"/>
+      <c r="E3" s="218" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="225" t="s">
-        <v>192</v>
-      </c>
-      <c r="G3" s="226"/>
-      <c r="H3" s="261"/>
-      <c r="I3" s="261"/>
-      <c r="J3" s="261"/>
-      <c r="K3" s="261"/>
-      <c r="L3" s="261"/>
-      <c r="M3" s="261"/>
-      <c r="N3" s="261"/>
-      <c r="O3" s="261"/>
-      <c r="P3" s="261"/>
-      <c r="Q3" s="261"/>
-      <c r="R3" s="261"/>
-      <c r="S3" s="261"/>
-      <c r="T3" s="261"/>
-      <c r="U3" s="261"/>
-      <c r="V3" s="261"/>
-    </row>
-    <row r="4" spans="1:22" ht="24">
-      <c r="A4" s="261"/>
-      <c r="B4" s="278" t="s">
+      <c r="F3" s="283" t="s">
+        <v>191</v>
+      </c>
+      <c r="G3" s="284"/>
+      <c r="H3" s="199"/>
+      <c r="I3" s="199"/>
+      <c r="J3" s="199"/>
+      <c r="K3" s="199"/>
+      <c r="L3" s="199"/>
+      <c r="M3" s="199"/>
+      <c r="N3" s="199"/>
+      <c r="O3" s="199"/>
+      <c r="P3" s="199"/>
+      <c r="Q3" s="199"/>
+      <c r="R3" s="199"/>
+      <c r="S3" s="199"/>
+      <c r="T3" s="199"/>
+      <c r="U3" s="199"/>
+      <c r="V3" s="199"/>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="199"/>
+      <c r="B4" s="216" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="227" t="s">
+      <c r="C4" s="285" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="229"/>
-      <c r="E4" s="280" t="s">
+      <c r="D4" s="287"/>
+      <c r="E4" s="218" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="226"/>
-      <c r="H4" s="261"/>
-      <c r="I4" s="261"/>
-      <c r="J4" s="261"/>
-      <c r="K4" s="261"/>
-      <c r="L4" s="261"/>
-      <c r="M4" s="261"/>
-      <c r="N4" s="261"/>
-      <c r="O4" s="261"/>
-      <c r="P4" s="261"/>
-      <c r="Q4" s="261"/>
-      <c r="R4" s="261"/>
-      <c r="S4" s="261"/>
-      <c r="T4" s="261"/>
-      <c r="U4" s="261"/>
-      <c r="V4" s="261"/>
-    </row>
-    <row r="5" spans="1:22" ht="36">
-      <c r="A5" s="261"/>
-      <c r="B5" s="278" t="s">
+      <c r="F4" s="285"/>
+      <c r="G4" s="284"/>
+      <c r="H4" s="199"/>
+      <c r="I4" s="199"/>
+      <c r="J4" s="199"/>
+      <c r="K4" s="199"/>
+      <c r="L4" s="199"/>
+      <c r="M4" s="199"/>
+      <c r="N4" s="199"/>
+      <c r="O4" s="199"/>
+      <c r="P4" s="199"/>
+      <c r="Q4" s="199"/>
+      <c r="R4" s="199"/>
+      <c r="S4" s="199"/>
+      <c r="T4" s="199"/>
+      <c r="U4" s="199"/>
+      <c r="V4" s="199"/>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="199"/>
+      <c r="B5" s="216" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="285" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="287"/>
+      <c r="E5" s="218"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="284"/>
+      <c r="H5" s="199"/>
+      <c r="I5" s="199"/>
+      <c r="J5" s="199"/>
+      <c r="K5" s="199"/>
+      <c r="L5" s="199"/>
+      <c r="M5" s="199"/>
+      <c r="N5" s="199"/>
+      <c r="O5" s="199"/>
+      <c r="P5" s="199"/>
+      <c r="Q5" s="199"/>
+      <c r="R5" s="199"/>
+      <c r="S5" s="199"/>
+      <c r="T5" s="199"/>
+      <c r="U5" s="199"/>
+      <c r="V5" s="199"/>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="199"/>
+      <c r="B6" s="216" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="285" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="229"/>
-      <c r="E5" s="280"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="226"/>
-      <c r="H5" s="261"/>
-      <c r="I5" s="261"/>
-      <c r="J5" s="261"/>
-      <c r="K5" s="261"/>
-      <c r="L5" s="261"/>
-      <c r="M5" s="261"/>
-      <c r="N5" s="261"/>
-      <c r="O5" s="261"/>
-      <c r="P5" s="261"/>
-      <c r="Q5" s="261"/>
-      <c r="R5" s="261"/>
-      <c r="S5" s="261"/>
-      <c r="T5" s="261"/>
-      <c r="U5" s="261"/>
-      <c r="V5" s="261"/>
-    </row>
-    <row r="6" spans="1:22" ht="36">
-      <c r="A6" s="261"/>
-      <c r="B6" s="278" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="227" t="s">
+      <c r="D6" s="287"/>
+      <c r="E6" s="219"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="284"/>
+      <c r="H6" s="199"/>
+      <c r="I6" s="199"/>
+      <c r="J6" s="199"/>
+      <c r="K6" s="199"/>
+      <c r="L6" s="199"/>
+      <c r="M6" s="199"/>
+      <c r="N6" s="199"/>
+      <c r="O6" s="199"/>
+      <c r="P6" s="199"/>
+      <c r="Q6" s="199"/>
+      <c r="R6" s="199"/>
+      <c r="S6" s="199"/>
+      <c r="T6" s="199"/>
+      <c r="U6" s="199"/>
+      <c r="V6" s="199"/>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="199"/>
+      <c r="B7" s="269" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="270"/>
+      <c r="D7" s="270"/>
+      <c r="E7" s="270"/>
+      <c r="F7" s="270"/>
+      <c r="G7" s="271"/>
+      <c r="H7" s="199"/>
+      <c r="I7" s="199"/>
+      <c r="J7" s="199"/>
+      <c r="K7" s="199"/>
+      <c r="L7" s="199"/>
+      <c r="M7" s="199"/>
+      <c r="N7" s="199"/>
+      <c r="O7" s="199"/>
+      <c r="P7" s="199"/>
+      <c r="Q7" s="199"/>
+      <c r="R7" s="199"/>
+      <c r="S7" s="199"/>
+      <c r="T7" s="199"/>
+      <c r="U7" s="199"/>
+      <c r="V7" s="199"/>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="199"/>
+      <c r="B8" s="272"/>
+      <c r="C8" s="273"/>
+      <c r="D8" s="273"/>
+      <c r="E8" s="273"/>
+      <c r="F8" s="273"/>
+      <c r="G8" s="274"/>
+      <c r="H8" s="199"/>
+      <c r="I8" s="199"/>
+      <c r="J8" s="199"/>
+      <c r="K8" s="199"/>
+      <c r="L8" s="199"/>
+      <c r="M8" s="199"/>
+      <c r="N8" s="199"/>
+      <c r="O8" s="199"/>
+      <c r="P8" s="199"/>
+      <c r="Q8" s="199"/>
+      <c r="R8" s="199"/>
+      <c r="S8" s="199"/>
+      <c r="T8" s="199"/>
+      <c r="U8" s="199"/>
+      <c r="V8" s="199"/>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="199"/>
+      <c r="B9" s="275"/>
+      <c r="C9" s="273"/>
+      <c r="D9" s="273"/>
+      <c r="E9" s="273"/>
+      <c r="F9" s="273"/>
+      <c r="G9" s="274"/>
+      <c r="H9" s="199"/>
+      <c r="I9" s="199"/>
+      <c r="J9" s="199"/>
+      <c r="K9" s="199"/>
+      <c r="L9" s="199"/>
+      <c r="M9" s="199"/>
+      <c r="N9" s="199"/>
+      <c r="O9" s="199"/>
+      <c r="P9" s="199"/>
+      <c r="Q9" s="199"/>
+      <c r="R9" s="199"/>
+      <c r="S9" s="199"/>
+      <c r="T9" s="199"/>
+      <c r="U9" s="199"/>
+      <c r="V9" s="199"/>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A10" s="199"/>
+      <c r="B10" s="276"/>
+      <c r="C10" s="277"/>
+      <c r="D10" s="277"/>
+      <c r="E10" s="277"/>
+      <c r="F10" s="277"/>
+      <c r="G10" s="278"/>
+      <c r="H10" s="199"/>
+      <c r="I10" s="199"/>
+      <c r="J10" s="199"/>
+      <c r="K10" s="199"/>
+      <c r="L10" s="199"/>
+      <c r="M10" s="199"/>
+      <c r="N10" s="199"/>
+      <c r="O10" s="199"/>
+      <c r="P10" s="199"/>
+      <c r="Q10" s="199"/>
+      <c r="R10" s="199"/>
+      <c r="S10" s="199"/>
+      <c r="T10" s="199"/>
+      <c r="U10" s="199"/>
+      <c r="V10" s="199"/>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A12" s="200" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="199"/>
+      <c r="C12" s="199"/>
+      <c r="D12" s="199"/>
+      <c r="E12" s="199"/>
+      <c r="F12" s="199"/>
+      <c r="G12" s="199"/>
+      <c r="H12" s="199"/>
+      <c r="I12" s="199"/>
+      <c r="J12" s="199"/>
+      <c r="K12" s="199"/>
+      <c r="L12" s="199"/>
+      <c r="M12" s="199"/>
+      <c r="N12" s="199"/>
+      <c r="O12" s="199"/>
+      <c r="P12" s="199"/>
+      <c r="Q12" s="199"/>
+      <c r="R12" s="199"/>
+      <c r="S12" s="199"/>
+      <c r="T12" s="199"/>
+      <c r="U12" s="199"/>
+      <c r="V12" s="199"/>
+    </row>
+    <row r="13" spans="1:22" ht="24">
+      <c r="A13" s="206" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="207" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="207" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="207" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="208" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="207" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="209" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="248"/>
+      <c r="M13" s="253"/>
+      <c r="N13" s="253"/>
+      <c r="O13" s="253"/>
+      <c r="P13" s="237"/>
+      <c r="Q13" s="237"/>
+      <c r="R13" s="237"/>
+      <c r="S13" s="237"/>
+      <c r="T13" s="237"/>
+      <c r="U13" s="237"/>
+      <c r="V13" s="237"/>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" s="225">
+        <v>2</v>
+      </c>
+      <c r="B14" s="226" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" s="227" t="s">
         <v>181</v>
       </c>
-      <c r="D6" s="229"/>
-      <c r="E6" s="281"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="226"/>
-      <c r="H6" s="261"/>
-      <c r="I6" s="261"/>
-      <c r="J6" s="261"/>
-      <c r="K6" s="261"/>
-      <c r="L6" s="261"/>
-      <c r="M6" s="261"/>
-      <c r="N6" s="261"/>
-      <c r="O6" s="261"/>
-      <c r="P6" s="261"/>
-      <c r="Q6" s="261"/>
-      <c r="R6" s="261"/>
-      <c r="S6" s="261"/>
-      <c r="T6" s="261"/>
-      <c r="U6" s="261"/>
-      <c r="V6" s="261"/>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="261"/>
-      <c r="B7" s="211" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="212"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="213"/>
-      <c r="H7" s="261"/>
-      <c r="I7" s="261"/>
-      <c r="J7" s="261"/>
-      <c r="K7" s="261"/>
-      <c r="L7" s="261"/>
-      <c r="M7" s="261"/>
-      <c r="N7" s="261"/>
-      <c r="O7" s="261"/>
-      <c r="P7" s="261"/>
-      <c r="Q7" s="261"/>
-      <c r="R7" s="261"/>
-      <c r="S7" s="261"/>
-      <c r="T7" s="261"/>
-      <c r="U7" s="261"/>
-      <c r="V7" s="261"/>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="261"/>
-      <c r="B8" s="214"/>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
-      <c r="H8" s="261"/>
-      <c r="I8" s="261"/>
-      <c r="J8" s="261"/>
-      <c r="K8" s="261"/>
-      <c r="L8" s="261"/>
-      <c r="M8" s="261"/>
-      <c r="N8" s="261"/>
-      <c r="O8" s="261"/>
-      <c r="P8" s="261"/>
-      <c r="Q8" s="261"/>
-      <c r="R8" s="261"/>
-      <c r="S8" s="261"/>
-      <c r="T8" s="261"/>
-      <c r="U8" s="261"/>
-      <c r="V8" s="261"/>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="261"/>
-      <c r="B9" s="217"/>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="216"/>
-      <c r="H9" s="261"/>
-      <c r="I9" s="261"/>
-      <c r="J9" s="261"/>
-      <c r="K9" s="261"/>
-      <c r="L9" s="261"/>
-      <c r="M9" s="261"/>
-      <c r="N9" s="261"/>
-      <c r="O9" s="261"/>
-      <c r="P9" s="261"/>
-      <c r="Q9" s="261"/>
-      <c r="R9" s="261"/>
-      <c r="S9" s="261"/>
-      <c r="T9" s="261"/>
-      <c r="U9" s="261"/>
-      <c r="V9" s="261"/>
-    </row>
-    <row r="10" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A10" s="261"/>
-      <c r="B10" s="218"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="220"/>
-      <c r="H10" s="261"/>
-      <c r="I10" s="261"/>
-      <c r="J10" s="261"/>
-      <c r="K10" s="261"/>
-      <c r="L10" s="261"/>
-      <c r="M10" s="261"/>
-      <c r="N10" s="261"/>
-      <c r="O10" s="261"/>
-      <c r="P10" s="261"/>
-      <c r="Q10" s="261"/>
-      <c r="R10" s="261"/>
-      <c r="S10" s="261"/>
-      <c r="T10" s="261"/>
-      <c r="U10" s="261"/>
-      <c r="V10" s="261"/>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A12" s="262" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="261"/>
-      <c r="C12" s="261"/>
-      <c r="D12" s="261"/>
-      <c r="E12" s="261"/>
-      <c r="F12" s="261"/>
-      <c r="G12" s="261"/>
-      <c r="H12" s="261"/>
-      <c r="I12" s="261"/>
-      <c r="J12" s="261"/>
-      <c r="K12" s="261"/>
-      <c r="L12" s="261"/>
-      <c r="M12" s="261"/>
-      <c r="N12" s="261"/>
-      <c r="O12" s="261"/>
-      <c r="P12" s="261"/>
-      <c r="Q12" s="261"/>
-      <c r="R12" s="261"/>
-      <c r="S12" s="261"/>
-      <c r="T12" s="261"/>
-      <c r="U12" s="261"/>
-      <c r="V12" s="261"/>
-    </row>
-    <row r="13" spans="1:22" ht="24">
-      <c r="A13" s="268" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="269" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="269" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="269" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="270" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="269" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="271" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="310"/>
-      <c r="M13" s="315"/>
-      <c r="N13" s="315"/>
-      <c r="O13" s="315"/>
-      <c r="P13" s="299"/>
-      <c r="Q13" s="299"/>
-      <c r="R13" s="299"/>
-      <c r="S13" s="299"/>
-      <c r="T13" s="299"/>
-      <c r="U13" s="299"/>
-      <c r="V13" s="299"/>
-    </row>
-    <row r="14" spans="1:22">
-      <c r="A14" s="287">
-        <v>2</v>
-      </c>
-      <c r="B14" s="288" t="s">
-        <v>186</v>
-      </c>
-      <c r="C14" s="289" t="s">
+      <c r="D14" s="227" t="s">
+        <v>196</v>
+      </c>
+      <c r="E14" s="228" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="229"/>
+      <c r="G14" s="233"/>
+      <c r="H14" s="252"/>
+      <c r="M14" s="238"/>
+      <c r="N14" s="238"/>
+      <c r="O14" s="237"/>
+      <c r="P14" s="237"/>
+      <c r="Q14" s="237"/>
+      <c r="R14" s="237"/>
+      <c r="S14" s="237"/>
+      <c r="T14" s="237"/>
+      <c r="U14" s="237"/>
+      <c r="V14" s="237"/>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A15" s="225">
+        <v>3</v>
+      </c>
+      <c r="B15" s="226" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" s="227" t="s">
+        <v>188</v>
+      </c>
+      <c r="D15" s="227" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" s="228"/>
+      <c r="F15" s="229"/>
+      <c r="G15" s="234"/>
+      <c r="H15" s="248"/>
+      <c r="I15" s="237"/>
+      <c r="J15" s="237"/>
+      <c r="K15" s="237"/>
+      <c r="L15" s="237"/>
+      <c r="M15" s="237"/>
+      <c r="N15" s="237"/>
+      <c r="O15" s="237"/>
+      <c r="P15" s="237"/>
+      <c r="Q15" s="237"/>
+      <c r="R15" s="237"/>
+      <c r="S15" s="237"/>
+      <c r="T15" s="237"/>
+      <c r="U15" s="237"/>
+      <c r="V15" s="237"/>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="225">
+        <v>4</v>
+      </c>
+      <c r="B16" s="226" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16" s="244" t="s">
         <v>182</v>
       </c>
-      <c r="D14" s="177" t="s">
-        <v>155</v>
-      </c>
-      <c r="E14" s="290" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="291"/>
-      <c r="G14" s="295"/>
-      <c r="H14" s="314"/>
-      <c r="M14" s="300"/>
-      <c r="N14" s="300"/>
-      <c r="O14" s="299"/>
-      <c r="P14" s="299"/>
-      <c r="Q14" s="299"/>
-      <c r="R14" s="299"/>
-      <c r="S14" s="299"/>
-      <c r="T14" s="299"/>
-      <c r="U14" s="299"/>
-      <c r="V14" s="299"/>
-    </row>
-    <row r="15" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A15" s="287">
-        <v>3</v>
-      </c>
-      <c r="B15" s="288" t="s">
-        <v>145</v>
-      </c>
-      <c r="C15" s="289" t="s">
-        <v>189</v>
-      </c>
-      <c r="D15" s="289" t="s">
-        <v>152</v>
-      </c>
-      <c r="E15" s="290"/>
-      <c r="F15" s="291"/>
-      <c r="G15" s="296"/>
-      <c r="H15" s="310"/>
-      <c r="I15" s="299"/>
-      <c r="J15" s="299"/>
-      <c r="K15" s="299"/>
-      <c r="L15" s="299"/>
-      <c r="M15" s="299"/>
-      <c r="N15" s="299"/>
-      <c r="O15" s="299"/>
-      <c r="P15" s="299"/>
-      <c r="Q15" s="299"/>
-      <c r="R15" s="299"/>
-      <c r="S15" s="299"/>
-      <c r="T15" s="299"/>
-      <c r="U15" s="299"/>
-      <c r="V15" s="299"/>
-    </row>
-    <row r="16" spans="1:22">
-      <c r="A16" s="287">
-        <v>4</v>
-      </c>
-      <c r="B16" s="288" t="s">
+      <c r="D16" s="235" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" s="228"/>
+      <c r="F16" s="229"/>
+      <c r="G16" s="232"/>
+      <c r="H16" s="248"/>
+      <c r="I16" s="249" t="s">
+        <v>181</v>
+      </c>
+      <c r="J16" s="249" t="s">
+        <v>139</v>
+      </c>
+      <c r="K16" s="249" t="s">
+        <v>182</v>
+      </c>
+      <c r="L16" s="245" t="s">
+        <v>183</v>
+      </c>
+      <c r="M16" s="237"/>
+      <c r="N16" s="237"/>
+      <c r="O16" s="237"/>
+      <c r="P16" s="237"/>
+      <c r="Q16" s="237"/>
+      <c r="R16" s="237"/>
+      <c r="S16" s="237"/>
+      <c r="T16" s="237"/>
+      <c r="U16" s="237"/>
+      <c r="V16" s="237"/>
+    </row>
+    <row r="17" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A17" s="231">
+        <v>5</v>
+      </c>
+      <c r="B17" s="239" t="s">
         <v>190</v>
       </c>
-      <c r="C16" s="306" t="s">
-        <v>183</v>
-      </c>
-      <c r="D16" s="297" t="s">
-        <v>152</v>
-      </c>
-      <c r="E16" s="290"/>
-      <c r="F16" s="291"/>
-      <c r="G16" s="294"/>
-      <c r="H16" s="310"/>
-      <c r="I16" s="311" t="s">
-        <v>182</v>
-      </c>
-      <c r="J16" s="311" t="s">
-        <v>140</v>
-      </c>
-      <c r="K16" s="311" t="s">
-        <v>183</v>
-      </c>
-      <c r="L16" s="307" t="s">
-        <v>184</v>
-      </c>
-      <c r="M16" s="299"/>
-      <c r="N16" s="299"/>
-      <c r="O16" s="299"/>
-      <c r="P16" s="299"/>
-      <c r="Q16" s="299"/>
-      <c r="R16" s="299"/>
-      <c r="S16" s="299"/>
-      <c r="T16" s="299"/>
-      <c r="U16" s="299"/>
-      <c r="V16" s="299"/>
-    </row>
-    <row r="17" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A17" s="293">
-        <v>5</v>
-      </c>
-      <c r="B17" s="301" t="s">
-        <v>191</v>
-      </c>
-      <c r="C17" s="292" t="s">
-        <v>159</v>
+      <c r="C17" s="230" t="s">
+        <v>158</v>
       </c>
       <c r="D17" s="158" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="302"/>
-      <c r="F17" s="303"/>
-      <c r="G17" s="304"/>
-      <c r="H17" s="310"/>
-      <c r="I17" s="308" t="s">
-        <v>185</v>
-      </c>
-      <c r="J17" s="312">
+      <c r="E17" s="240"/>
+      <c r="F17" s="241"/>
+      <c r="G17" s="242"/>
+      <c r="H17" s="248"/>
+      <c r="I17" s="246" t="s">
+        <v>184</v>
+      </c>
+      <c r="J17" s="250">
         <v>40901</v>
       </c>
-      <c r="K17" s="312">
+      <c r="K17" s="250">
         <v>40902</v>
       </c>
-      <c r="L17" s="316">
+      <c r="L17" s="254">
         <v>1</v>
       </c>
-      <c r="M17" s="299"/>
-      <c r="N17" s="299"/>
-      <c r="O17" s="299"/>
-      <c r="P17" s="299"/>
-      <c r="Q17" s="299"/>
-      <c r="R17" s="299"/>
-      <c r="S17" s="299"/>
-      <c r="T17" s="299"/>
-      <c r="U17" s="299"/>
-      <c r="V17" s="299"/>
+      <c r="M17" s="237"/>
+      <c r="N17" s="237"/>
+      <c r="O17" s="237"/>
+      <c r="P17" s="237"/>
+      <c r="Q17" s="237"/>
+      <c r="R17" s="237"/>
+      <c r="S17" s="237"/>
+      <c r="T17" s="237"/>
+      <c r="U17" s="237"/>
+      <c r="V17" s="237"/>
     </row>
     <row r="18" spans="1:22" ht="15.75" thickBot="1">
-      <c r="I18" s="309" t="s">
+      <c r="I18" s="247" t="s">
+        <v>186</v>
+      </c>
+      <c r="J18" s="247" t="s">
         <v>187</v>
       </c>
-      <c r="J18" s="309" t="s">
-        <v>188</v>
-      </c>
-      <c r="K18" s="313">
+      <c r="K18" s="251">
         <v>40493</v>
       </c>
-      <c r="L18" s="317">
+      <c r="L18" s="255">
         <v>41255</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A19" s="262" t="s">
+      <c r="A19" s="200" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="261"/>
-      <c r="C19" s="261"/>
-      <c r="D19" s="261"/>
-      <c r="E19" s="261"/>
-      <c r="F19" s="261"/>
-      <c r="G19" s="261"/>
-      <c r="H19" s="261"/>
-      <c r="I19" s="261"/>
-      <c r="J19" s="261"/>
-      <c r="K19" s="261"/>
-      <c r="L19" s="261"/>
-      <c r="M19" s="261"/>
-      <c r="N19" s="261"/>
-      <c r="O19" s="261"/>
-      <c r="P19" s="261"/>
-      <c r="Q19" s="261"/>
-      <c r="R19" s="261"/>
-      <c r="S19" s="261"/>
-      <c r="T19" s="261"/>
-      <c r="U19" s="261"/>
-      <c r="V19" s="261"/>
+      <c r="B19" s="199"/>
+      <c r="C19" s="199"/>
+      <c r="D19" s="199"/>
+      <c r="E19" s="199"/>
+      <c r="F19" s="199"/>
+      <c r="G19" s="199"/>
+      <c r="H19" s="199"/>
+      <c r="I19" s="199"/>
+      <c r="J19" s="199"/>
+      <c r="K19" s="199"/>
+      <c r="L19" s="199"/>
+      <c r="M19" s="199"/>
+      <c r="N19" s="199"/>
+      <c r="O19" s="199"/>
+      <c r="P19" s="199"/>
+      <c r="Q19" s="199"/>
+      <c r="R19" s="199"/>
+      <c r="S19" s="199"/>
+      <c r="T19" s="199"/>
+      <c r="U19" s="199"/>
+      <c r="V19" s="199"/>
     </row>
     <row r="20" spans="1:22">
-      <c r="A20" s="267" t="s">
+      <c r="A20" s="205" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="272" t="s">
+      <c r="B20" s="210" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="209" t="s">
+      <c r="C20" s="267" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="210"/>
-      <c r="E20" s="272" t="s">
+      <c r="D20" s="268"/>
+      <c r="E20" s="210" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="272" t="s">
+      <c r="F20" s="210" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="273" t="s">
+      <c r="G20" s="211" t="s">
         <v>31</v>
       </c>
-      <c r="H20" s="261"/>
-      <c r="I20" s="261"/>
-      <c r="J20" s="261"/>
-      <c r="K20" s="261"/>
-      <c r="L20" s="261"/>
-      <c r="M20" s="261"/>
-      <c r="N20" s="261"/>
-      <c r="O20" s="261"/>
-      <c r="P20" s="261"/>
-      <c r="Q20" s="261"/>
-      <c r="R20" s="261"/>
-      <c r="S20" s="261"/>
-      <c r="T20" s="261"/>
-      <c r="U20" s="261"/>
-      <c r="V20" s="261"/>
+      <c r="H20" s="199"/>
+      <c r="I20" s="199"/>
+      <c r="J20" s="199"/>
+      <c r="K20" s="199"/>
+      <c r="L20" s="199"/>
+      <c r="M20" s="199"/>
+      <c r="N20" s="199"/>
+      <c r="O20" s="199"/>
+      <c r="P20" s="199"/>
+      <c r="Q20" s="199"/>
+      <c r="R20" s="199"/>
+      <c r="S20" s="199"/>
+      <c r="T20" s="199"/>
+      <c r="U20" s="199"/>
+      <c r="V20" s="199"/>
     </row>
     <row r="21" spans="1:22">
-      <c r="A21" s="264">
+      <c r="A21" s="202">
         <v>1</v>
       </c>
-      <c r="B21" s="265" t="s">
+      <c r="B21" s="203" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="249" t="s">
+      <c r="C21" s="303" t="s">
+        <v>193</v>
+      </c>
+      <c r="D21" s="304"/>
+      <c r="E21" s="220" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="220" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="204"/>
+      <c r="H21" s="199"/>
+      <c r="I21" s="199"/>
+      <c r="J21" s="199"/>
+      <c r="K21" s="199"/>
+      <c r="L21" s="199"/>
+      <c r="M21" s="199"/>
+      <c r="N21" s="199"/>
+      <c r="O21" s="199"/>
+      <c r="P21" s="199"/>
+      <c r="Q21" s="199"/>
+      <c r="R21" s="199"/>
+      <c r="S21" s="199"/>
+      <c r="T21" s="199"/>
+      <c r="U21" s="199"/>
+      <c r="V21" s="199"/>
+    </row>
+    <row r="22" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A22" s="223">
+        <v>2</v>
+      </c>
+      <c r="B22" s="221" t="s">
         <v>194</v>
       </c>
-      <c r="D21" s="250"/>
-      <c r="E21" s="282" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="282" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="266"/>
-      <c r="H21" s="261"/>
-      <c r="I21" s="261"/>
-      <c r="J21" s="261"/>
-      <c r="K21" s="261"/>
-      <c r="L21" s="261"/>
-      <c r="M21" s="261"/>
-      <c r="N21" s="261"/>
-      <c r="O21" s="261"/>
-      <c r="P21" s="261"/>
-      <c r="Q21" s="261"/>
-      <c r="R21" s="261"/>
-      <c r="S21" s="261"/>
-      <c r="T21" s="261"/>
-      <c r="U21" s="261"/>
-      <c r="V21" s="261"/>
-    </row>
-    <row r="22" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A22" s="285">
-        <v>2</v>
-      </c>
-      <c r="B22" s="283" t="s">
+      <c r="C22" s="305" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" s="306"/>
+      <c r="E22" s="224"/>
+      <c r="F22" s="224"/>
+      <c r="G22" s="222"/>
+      <c r="H22" s="199"/>
+      <c r="I22" s="199"/>
+      <c r="J22" s="199"/>
+      <c r="K22" s="199"/>
+      <c r="L22" s="199"/>
+      <c r="M22" s="199"/>
+      <c r="N22" s="199"/>
+      <c r="O22" s="199"/>
+      <c r="P22" s="199"/>
+      <c r="Q22" s="199"/>
+      <c r="R22" s="199"/>
+      <c r="S22" s="199"/>
+      <c r="T22" s="199"/>
+      <c r="U22" s="199"/>
+      <c r="V22" s="199"/>
+    </row>
+    <row r="24" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A24" s="200" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="199"/>
+      <c r="C24" s="199"/>
+      <c r="D24" s="199"/>
+      <c r="E24" s="199"/>
+      <c r="F24" s="199"/>
+      <c r="G24" s="199"/>
+      <c r="H24" s="199"/>
+      <c r="I24" s="199"/>
+      <c r="J24" s="199"/>
+      <c r="K24" s="199"/>
+      <c r="L24" s="199"/>
+      <c r="M24" s="199"/>
+      <c r="N24" s="199"/>
+      <c r="O24" s="199"/>
+      <c r="P24" s="199"/>
+      <c r="Q24" s="199"/>
+      <c r="R24" s="199"/>
+      <c r="S24" s="199"/>
+      <c r="T24" s="199"/>
+      <c r="U24" s="199"/>
+      <c r="V24" s="199"/>
+    </row>
+    <row r="25" spans="1:22" ht="24.75" thickBot="1">
+      <c r="A25" s="212" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="213" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="260" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="261"/>
+      <c r="E25" s="260" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="262"/>
+      <c r="G25" s="214" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="199"/>
+      <c r="I25" s="199"/>
+      <c r="J25" s="199"/>
+      <c r="K25" s="199"/>
+      <c r="L25" s="199"/>
+      <c r="M25" s="199"/>
+      <c r="N25" s="199"/>
+      <c r="O25" s="199"/>
+      <c r="P25" s="199"/>
+      <c r="Q25" s="199"/>
+      <c r="R25" s="199"/>
+      <c r="S25" s="199"/>
+      <c r="T25" s="199"/>
+      <c r="U25" s="199"/>
+      <c r="V25" s="199"/>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="A26" s="201">
+        <v>1</v>
+      </c>
+      <c r="B26" s="198" t="s">
         <v>195</v>
       </c>
-      <c r="C22" s="247" t="s">
-        <v>171</v>
-      </c>
-      <c r="D22" s="248"/>
-      <c r="E22" s="286"/>
-      <c r="F22" s="286"/>
-      <c r="G22" s="284"/>
-      <c r="H22" s="261"/>
-      <c r="I22" s="261"/>
-      <c r="J22" s="261"/>
-      <c r="K22" s="261"/>
-      <c r="L22" s="261"/>
-      <c r="M22" s="261"/>
-      <c r="N22" s="261"/>
-      <c r="O22" s="261"/>
-      <c r="P22" s="261"/>
-      <c r="Q22" s="261"/>
-      <c r="R22" s="261"/>
-      <c r="S22" s="261"/>
-      <c r="T22" s="261"/>
-      <c r="U22" s="261"/>
-      <c r="V22" s="261"/>
-    </row>
-    <row r="24" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A24" s="262" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="261"/>
-      <c r="C24" s="261"/>
-      <c r="D24" s="261"/>
-      <c r="E24" s="261"/>
-      <c r="F24" s="261"/>
-      <c r="G24" s="261"/>
-      <c r="H24" s="261"/>
-      <c r="I24" s="261"/>
-      <c r="J24" s="261"/>
-      <c r="K24" s="261"/>
-      <c r="L24" s="261"/>
-      <c r="M24" s="261"/>
-      <c r="N24" s="261"/>
-      <c r="O24" s="261"/>
-      <c r="P24" s="261"/>
-      <c r="Q24" s="261"/>
-      <c r="R24" s="261"/>
-      <c r="S24" s="261"/>
-      <c r="T24" s="261"/>
-      <c r="U24" s="261"/>
-      <c r="V24" s="261"/>
-    </row>
-    <row r="25" spans="1:22" ht="24.75" thickBot="1">
-      <c r="A25" s="274" t="s">
+      <c r="C26" s="308" t="s">
+        <v>158</v>
+      </c>
+      <c r="D26" s="309"/>
+      <c r="E26" s="307" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="307"/>
+      <c r="G26" s="236" t="s">
+        <v>114</v>
+      </c>
+      <c r="H26" s="199"/>
+      <c r="I26" s="199"/>
+      <c r="J26" s="199"/>
+      <c r="K26" s="199"/>
+      <c r="L26" s="199"/>
+      <c r="M26" s="199"/>
+      <c r="N26" s="199"/>
+      <c r="O26" s="199"/>
+      <c r="P26" s="199"/>
+      <c r="Q26" s="199"/>
+      <c r="R26" s="199"/>
+      <c r="S26" s="199"/>
+      <c r="T26" s="199"/>
+      <c r="U26" s="199"/>
+      <c r="V26" s="199"/>
+    </row>
+    <row r="27" spans="1:22">
+      <c r="A27" s="199"/>
+      <c r="B27" s="199"/>
+      <c r="C27" s="243"/>
+      <c r="D27" s="243"/>
+      <c r="E27" s="243"/>
+      <c r="F27" s="243"/>
+      <c r="G27" s="199"/>
+      <c r="H27" s="199"/>
+      <c r="I27" s="199"/>
+      <c r="J27" s="199"/>
+      <c r="K27" s="199"/>
+      <c r="L27" s="199"/>
+      <c r="M27" s="199"/>
+      <c r="N27" s="199"/>
+      <c r="O27" s="199"/>
+      <c r="P27" s="199"/>
+      <c r="Q27" s="199"/>
+      <c r="R27" s="199"/>
+      <c r="S27" s="199"/>
+      <c r="T27" s="199"/>
+      <c r="U27" s="199"/>
+      <c r="V27" s="199"/>
+    </row>
+    <row r="28" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A28" s="200" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="199"/>
+      <c r="C28" s="199"/>
+      <c r="D28" s="199"/>
+      <c r="E28" s="199"/>
+      <c r="F28" s="199"/>
+      <c r="G28" s="199"/>
+      <c r="H28" s="199"/>
+      <c r="I28" s="199"/>
+      <c r="J28" s="199"/>
+      <c r="K28" s="199"/>
+      <c r="L28" s="199"/>
+      <c r="M28" s="199"/>
+      <c r="N28" s="199"/>
+      <c r="O28" s="199"/>
+      <c r="P28" s="199"/>
+      <c r="Q28" s="199"/>
+      <c r="R28" s="199"/>
+      <c r="S28" s="199"/>
+      <c r="T28" s="199"/>
+      <c r="U28" s="199"/>
+      <c r="V28" s="199"/>
+    </row>
+    <row r="29" spans="1:22" ht="24.75" thickBot="1">
+      <c r="A29" s="212" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="275" t="s">
+      <c r="B29" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="202" t="s">
+      <c r="C29" s="260" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="203"/>
-      <c r="E25" s="202" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="204"/>
-      <c r="G25" s="276" t="s">
-        <v>38</v>
-      </c>
-      <c r="H25" s="261"/>
-      <c r="I25" s="261"/>
-      <c r="J25" s="261"/>
-      <c r="K25" s="261"/>
-      <c r="L25" s="261"/>
-      <c r="M25" s="261"/>
-      <c r="N25" s="261"/>
-      <c r="O25" s="261"/>
-      <c r="P25" s="261"/>
-      <c r="Q25" s="261"/>
-      <c r="R25" s="261"/>
-      <c r="S25" s="261"/>
-      <c r="T25" s="261"/>
-      <c r="U25" s="261"/>
-      <c r="V25" s="261"/>
-    </row>
-    <row r="26" spans="1:22">
-      <c r="A26" s="263">
-        <v>1</v>
-      </c>
-      <c r="B26" s="258" t="s">
-        <v>196</v>
-      </c>
-      <c r="C26" s="257" t="s">
-        <v>159</v>
-      </c>
-      <c r="D26" s="259"/>
-      <c r="E26" s="260" t="s">
-        <v>129</v>
-      </c>
-      <c r="F26" s="260"/>
-      <c r="G26" s="298" t="s">
-        <v>114</v>
-      </c>
-      <c r="H26" s="261"/>
-      <c r="I26" s="261"/>
-      <c r="J26" s="261"/>
-      <c r="K26" s="261"/>
-      <c r="L26" s="261"/>
-      <c r="M26" s="261"/>
-      <c r="N26" s="261"/>
-      <c r="O26" s="261"/>
-      <c r="P26" s="261"/>
-      <c r="Q26" s="261"/>
-      <c r="R26" s="261"/>
-      <c r="S26" s="261"/>
-      <c r="T26" s="261"/>
-      <c r="U26" s="261"/>
-      <c r="V26" s="261"/>
-    </row>
-    <row r="27" spans="1:22">
-      <c r="A27" s="261"/>
-      <c r="B27" s="261"/>
-      <c r="C27" s="305"/>
-      <c r="D27" s="305"/>
-      <c r="E27" s="305"/>
-      <c r="F27" s="305"/>
-      <c r="G27" s="261"/>
-      <c r="H27" s="261"/>
-      <c r="I27" s="261"/>
-      <c r="J27" s="261"/>
-      <c r="K27" s="261"/>
-      <c r="L27" s="261"/>
-      <c r="M27" s="261"/>
-      <c r="N27" s="261"/>
-      <c r="O27" s="261"/>
-      <c r="P27" s="261"/>
-      <c r="Q27" s="261"/>
-      <c r="R27" s="261"/>
-      <c r="S27" s="261"/>
-      <c r="T27" s="261"/>
-      <c r="U27" s="261"/>
-      <c r="V27" s="261"/>
-    </row>
-    <row r="28" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A28" s="262" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="261"/>
-      <c r="C28" s="261"/>
-      <c r="D28" s="261"/>
-      <c r="E28" s="261"/>
-      <c r="F28" s="261"/>
-      <c r="G28" s="261"/>
-      <c r="H28" s="261"/>
-      <c r="I28" s="261"/>
-      <c r="J28" s="261"/>
-      <c r="K28" s="261"/>
-      <c r="L28" s="261"/>
-      <c r="M28" s="261"/>
-      <c r="N28" s="261"/>
-      <c r="O28" s="261"/>
-      <c r="P28" s="261"/>
-      <c r="Q28" s="261"/>
-      <c r="R28" s="261"/>
-      <c r="S28" s="261"/>
-      <c r="T28" s="261"/>
-      <c r="U28" s="261"/>
-      <c r="V28" s="261"/>
-    </row>
-    <row r="29" spans="1:22" ht="48.75" thickBot="1">
-      <c r="A29" s="274" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="275" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="202" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" s="203"/>
-      <c r="E29" s="202" t="s">
+      <c r="D29" s="261"/>
+      <c r="E29" s="260" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="204"/>
-      <c r="G29" s="276" t="s">
+      <c r="F29" s="262"/>
+      <c r="G29" s="214" t="s">
         <v>39</v>
       </c>
     </row>
@@ -11139,103 +11173,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="281" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="228"/>
+      <c r="D2" s="286"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="223" t="s">
+      <c r="F2" s="281" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="224"/>
+      <c r="G2" s="282"/>
     </row>
     <row r="3" spans="1:11" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
+      <c r="C3" s="285"/>
+      <c r="D3" s="287"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="227" t="s">
+      <c r="F3" s="285" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="226"/>
+      <c r="G3" s="284"/>
     </row>
     <row r="4" spans="1:11" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="227" t="s">
+      <c r="C4" s="285" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="229"/>
+      <c r="D4" s="287"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="226"/>
+      <c r="F4" s="285"/>
+      <c r="G4" s="284"/>
     </row>
     <row r="5" spans="1:11" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="285" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="229"/>
+      <c r="D5" s="287"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="226"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="284"/>
     </row>
     <row r="6" spans="1:11" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="285" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="229"/>
+      <c r="D6" s="287"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="226"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="284"/>
     </row>
     <row r="7" spans="1:11" ht="14.25">
-      <c r="B7" s="211" t="s">
+      <c r="B7" s="269" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="212"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="213"/>
+      <c r="C7" s="270"/>
+      <c r="D7" s="270"/>
+      <c r="E7" s="270"/>
+      <c r="F7" s="270"/>
+      <c r="G7" s="271"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="B8" s="214"/>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
+      <c r="B8" s="272"/>
+      <c r="C8" s="273"/>
+      <c r="D8" s="273"/>
+      <c r="E8" s="273"/>
+      <c r="F8" s="273"/>
+      <c r="G8" s="274"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9" s="217"/>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="216"/>
+      <c r="B9" s="275"/>
+      <c r="C9" s="273"/>
+      <c r="D9" s="273"/>
+      <c r="E9" s="273"/>
+      <c r="F9" s="273"/>
+      <c r="G9" s="274"/>
     </row>
     <row r="10" spans="1:11" ht="12.75" thickBot="1">
-      <c r="B10" s="218"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="220"/>
+      <c r="B10" s="276"/>
+      <c r="C10" s="277"/>
+      <c r="D10" s="277"/>
+      <c r="E10" s="277"/>
+      <c r="F10" s="277"/>
+      <c r="G10" s="278"/>
     </row>
     <row r="12" spans="1:11" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -11457,10 +11491,10 @@
       <c r="B24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="209" t="s">
+      <c r="C24" s="267" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="210"/>
+      <c r="D24" s="268"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -11478,10 +11512,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="249" t="s">
+      <c r="C25" s="303" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="250"/>
+      <c r="D25" s="304"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -11495,10 +11529,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="54"/>
-      <c r="C26" s="247" t="s">
+      <c r="C26" s="305" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="248"/>
+      <c r="D26" s="306"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58" t="s">
         <v>3</v>
@@ -11517,14 +11551,14 @@
       <c r="B29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="202" t="s">
+      <c r="C29" s="260" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="203"/>
-      <c r="E29" s="202" t="s">
+      <c r="D29" s="261"/>
+      <c r="E29" s="260" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="204"/>
+      <c r="F29" s="262"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -11541,14 +11575,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="202" t="s">
+      <c r="C32" s="260" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="203"/>
-      <c r="E32" s="202" t="s">
+      <c r="D32" s="261"/>
+      <c r="E32" s="260" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="204"/>
+      <c r="F32" s="262"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -11558,14 +11592,14 @@
         <v>1</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="245" t="s">
+      <c r="C33" s="310" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="246"/>
-      <c r="E33" s="247" t="s">
+      <c r="D33" s="311"/>
+      <c r="E33" s="305" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="248"/>
+      <c r="F33" s="306"/>
       <c r="G33" s="28" t="s">
         <v>49</v>
       </c>
@@ -11640,105 +11674,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="281" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="228"/>
+      <c r="D2" s="286"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="223" t="s">
+      <c r="F2" s="281" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="224"/>
+      <c r="G2" s="282"/>
     </row>
     <row r="3" spans="1:7" ht="14.25">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
+      <c r="C3" s="285"/>
+      <c r="D3" s="287"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="227" t="s">
+      <c r="F3" s="285" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="226"/>
+      <c r="G3" s="284"/>
     </row>
     <row r="4" spans="1:7" ht="14.25">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="227" t="s">
+      <c r="C4" s="285" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="229"/>
+      <c r="D4" s="287"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="227"/>
-      <c r="G4" s="226"/>
+      <c r="F4" s="285"/>
+      <c r="G4" s="284"/>
     </row>
     <row r="5" spans="1:7" ht="24">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="285" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="229"/>
+      <c r="D5" s="287"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="226"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="284"/>
     </row>
     <row r="6" spans="1:7" ht="24">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="285" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="229"/>
+      <c r="D6" s="287"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="226"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="284"/>
     </row>
     <row r="7" spans="1:7" ht="14.25">
-      <c r="B7" s="211" t="s">
+      <c r="B7" s="269" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="212"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="213"/>
+      <c r="C7" s="270"/>
+      <c r="D7" s="270"/>
+      <c r="E7" s="270"/>
+      <c r="F7" s="270"/>
+      <c r="G7" s="271"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="214" t="s">
+      <c r="B8" s="272" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="215"/>
-      <c r="D8" s="215"/>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="216"/>
+      <c r="C8" s="273"/>
+      <c r="D8" s="273"/>
+      <c r="E8" s="273"/>
+      <c r="F8" s="273"/>
+      <c r="G8" s="274"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="217"/>
-      <c r="C9" s="215"/>
-      <c r="D9" s="215"/>
-      <c r="E9" s="215"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="216"/>
+      <c r="B9" s="275"/>
+      <c r="C9" s="273"/>
+      <c r="D9" s="273"/>
+      <c r="E9" s="273"/>
+      <c r="F9" s="273"/>
+      <c r="G9" s="274"/>
     </row>
     <row r="10" spans="1:7" ht="12.75" thickBot="1">
-      <c r="B10" s="218"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="220"/>
+      <c r="B10" s="276"/>
+      <c r="C10" s="277"/>
+      <c r="D10" s="277"/>
+      <c r="E10" s="277"/>
+      <c r="F10" s="277"/>
+      <c r="G10" s="278"/>
     </row>
     <row r="12" spans="1:7" ht="12.75" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -11843,10 +11877,10 @@
       <c r="B19" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="209" t="s">
+      <c r="C19" s="267" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="210"/>
+      <c r="D19" s="268"/>
       <c r="E19" s="34" t="s">
         <v>33</v>
       </c>
@@ -11864,10 +11898,10 @@
       <c r="B20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="249" t="s">
+      <c r="C20" s="303" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="250"/>
+      <c r="D20" s="304"/>
       <c r="E20" s="46" t="s">
         <v>3</v>
       </c>
@@ -11881,10 +11915,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="26"/>
-      <c r="C21" s="245" t="s">
+      <c r="C21" s="310" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="246"/>
+      <c r="D21" s="311"/>
       <c r="E21" s="45"/>
       <c r="F21" s="45" t="s">
         <v>3</v>
@@ -11903,14 +11937,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="202" t="s">
+      <c r="C24" s="260" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="203"/>
-      <c r="E24" s="202" t="s">
+      <c r="D24" s="261"/>
+      <c r="E24" s="260" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="204"/>
+      <c r="F24" s="262"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -11927,14 +11961,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="202" t="s">
+      <c r="C27" s="260" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="203"/>
-      <c r="E27" s="202" t="s">
+      <c r="D27" s="261"/>
+      <c r="E27" s="260" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="204"/>
+      <c r="F27" s="262"/>
       <c r="G27" s="38" t="s">
         <v>39</v>
       </c>
@@ -11944,10 +11978,10 @@
         <v>1</v>
       </c>
       <c r="B28" s="26"/>
-      <c r="C28" s="245"/>
-      <c r="D28" s="246"/>
-      <c r="E28" s="247"/>
-      <c r="F28" s="248"/>
+      <c r="C28" s="310"/>
+      <c r="D28" s="311"/>
+      <c r="E28" s="305"/>
+      <c r="F28" s="306"/>
       <c r="G28" s="28"/>
     </row>
   </sheetData>

</xml_diff>